<commit_message>
first version for John
</commit_message>
<xml_diff>
--- a/dataExpert.xlsx
+++ b/dataExpert.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/broche/Mon Drive/Docs/ResearchWorks/Moi - Indicateur Zoonoses/Analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/broche/Mon Drive/Docs/ResearchWorks/Moi - Indicateur Zoonoses/Analyse/WhoPrezodeIndicator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A301DB-019C-8043-B093-4F9ACE815ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A277A06C-F274-3040-A400-1470987768A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="338">
   <si>
     <t>participantId</t>
   </si>
@@ -1321,8 +1321,8 @@
   </sheetPr>
   <dimension ref="A1:N574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A557" workbookViewId="0">
-      <selection activeCell="M173" sqref="M173"/>
+    <sheetView tabSelected="1" topLeftCell="A502" workbookViewId="0">
+      <selection activeCell="J575" sqref="J575"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17544,8 +17544,8 @@
       <c r="E381" s="1">
         <v>4</v>
       </c>
-      <c r="F381" s="1" t="s">
-        <v>17</v>
+      <c r="F381" s="1">
+        <v>0</v>
       </c>
       <c r="G381" s="1">
         <v>1</v>
@@ -17556,8 +17556,8 @@
       <c r="I381" s="1">
         <v>4</v>
       </c>
-      <c r="J381" s="1" t="s">
-        <v>17</v>
+      <c r="J381" s="1">
+        <v>0</v>
       </c>
       <c r="K381" s="1">
         <v>1</v>
@@ -17588,8 +17588,8 @@
       <c r="E382" s="1">
         <v>4</v>
       </c>
-      <c r="F382" s="1" t="s">
-        <v>17</v>
+      <c r="F382" s="1">
+        <v>0</v>
       </c>
       <c r="G382" s="1">
         <v>1</v>
@@ -17600,8 +17600,8 @@
       <c r="I382" s="1">
         <v>4</v>
       </c>
-      <c r="J382" s="1" t="s">
-        <v>17</v>
+      <c r="J382" s="1">
+        <v>0</v>
       </c>
       <c r="K382" s="1">
         <v>1</v>
@@ -17632,8 +17632,8 @@
       <c r="E383" s="1">
         <v>4</v>
       </c>
-      <c r="F383" s="1" t="s">
-        <v>17</v>
+      <c r="F383" s="1">
+        <v>0</v>
       </c>
       <c r="G383" s="1">
         <v>1</v>
@@ -17644,8 +17644,8 @@
       <c r="I383" s="1">
         <v>4</v>
       </c>
-      <c r="J383" s="1" t="s">
-        <v>17</v>
+      <c r="J383" s="1">
+        <v>0</v>
       </c>
       <c r="K383" s="1">
         <v>1</v>
@@ -17676,8 +17676,8 @@
       <c r="E384" s="1">
         <v>4</v>
       </c>
-      <c r="F384" s="1" t="s">
-        <v>17</v>
+      <c r="F384" s="1">
+        <v>0</v>
       </c>
       <c r="G384" s="1">
         <v>1</v>
@@ -17688,8 +17688,8 @@
       <c r="I384" s="1">
         <v>4</v>
       </c>
-      <c r="J384" s="1" t="s">
-        <v>17</v>
+      <c r="J384" s="1">
+        <v>0</v>
       </c>
       <c r="K384" s="1">
         <v>1</v>
@@ -17720,8 +17720,8 @@
       <c r="E385" s="1">
         <v>4</v>
       </c>
-      <c r="F385" s="1" t="s">
-        <v>17</v>
+      <c r="F385" s="1">
+        <v>0</v>
       </c>
       <c r="G385" s="1">
         <v>1</v>
@@ -17732,8 +17732,8 @@
       <c r="I385" s="1">
         <v>4</v>
       </c>
-      <c r="J385" s="1" t="s">
-        <v>17</v>
+      <c r="J385" s="1">
+        <v>0</v>
       </c>
       <c r="K385" s="1">
         <v>1</v>
@@ -17764,8 +17764,8 @@
       <c r="E386" s="1">
         <v>4</v>
       </c>
-      <c r="F386" s="1" t="s">
-        <v>17</v>
+      <c r="F386" s="1">
+        <v>0</v>
       </c>
       <c r="G386" s="1">
         <v>1</v>
@@ -17776,8 +17776,8 @@
       <c r="I386" s="1">
         <v>4</v>
       </c>
-      <c r="J386" s="1" t="s">
-        <v>17</v>
+      <c r="J386" s="1">
+        <v>0</v>
       </c>
       <c r="K386" s="1">
         <v>1</v>
@@ -17808,8 +17808,8 @@
       <c r="E387" s="1">
         <v>4</v>
       </c>
-      <c r="F387" s="1" t="s">
-        <v>17</v>
+      <c r="F387" s="1">
+        <v>0</v>
       </c>
       <c r="G387" s="1">
         <v>1</v>
@@ -17820,8 +17820,8 @@
       <c r="I387" s="1">
         <v>4</v>
       </c>
-      <c r="J387" s="1" t="s">
-        <v>17</v>
+      <c r="J387" s="1">
+        <v>0</v>
       </c>
       <c r="K387" s="1">
         <v>1</v>
@@ -17852,8 +17852,8 @@
       <c r="E388" s="1">
         <v>4</v>
       </c>
-      <c r="F388" s="1" t="s">
-        <v>17</v>
+      <c r="F388" s="1">
+        <v>0</v>
       </c>
       <c r="G388" s="1">
         <v>1</v>
@@ -17864,8 +17864,8 @@
       <c r="I388" s="1">
         <v>4</v>
       </c>
-      <c r="J388" s="1" t="s">
-        <v>17</v>
+      <c r="J388" s="1">
+        <v>0</v>
       </c>
       <c r="K388" s="1">
         <v>1</v>
@@ -17896,8 +17896,8 @@
       <c r="E389" s="1">
         <v>4</v>
       </c>
-      <c r="F389" s="1" t="s">
-        <v>17</v>
+      <c r="F389" s="1">
+        <v>0</v>
       </c>
       <c r="G389" s="1">
         <v>1</v>
@@ -17908,8 +17908,8 @@
       <c r="I389" s="1">
         <v>4</v>
       </c>
-      <c r="J389" s="1" t="s">
-        <v>17</v>
+      <c r="J389" s="1">
+        <v>0</v>
       </c>
       <c r="K389" s="1">
         <v>1</v>
@@ -17940,8 +17940,8 @@
       <c r="E390" s="1">
         <v>4</v>
       </c>
-      <c r="F390" s="1" t="s">
-        <v>17</v>
+      <c r="F390" s="1">
+        <v>0</v>
       </c>
       <c r="G390" s="1">
         <v>1</v>
@@ -17952,8 +17952,8 @@
       <c r="I390" s="1">
         <v>4</v>
       </c>
-      <c r="J390" s="1" t="s">
-        <v>17</v>
+      <c r="J390" s="1">
+        <v>0</v>
       </c>
       <c r="K390" s="1">
         <v>1</v>
@@ -17984,8 +17984,8 @@
       <c r="E391" s="1">
         <v>4</v>
       </c>
-      <c r="F391" s="1" t="s">
-        <v>17</v>
+      <c r="F391" s="1">
+        <v>0</v>
       </c>
       <c r="G391" s="1">
         <v>1</v>
@@ -17996,8 +17996,8 @@
       <c r="I391" s="1">
         <v>4</v>
       </c>
-      <c r="J391" s="1" t="s">
-        <v>17</v>
+      <c r="J391" s="1">
+        <v>0</v>
       </c>
       <c r="K391" s="1">
         <v>1</v>
@@ -18028,8 +18028,8 @@
       <c r="E392" s="1">
         <v>4</v>
       </c>
-      <c r="F392" s="1" t="s">
-        <v>17</v>
+      <c r="F392" s="1">
+        <v>0</v>
       </c>
       <c r="G392" s="1">
         <v>1</v>
@@ -18040,8 +18040,8 @@
       <c r="I392" s="1">
         <v>4</v>
       </c>
-      <c r="J392" s="1" t="s">
-        <v>17</v>
+      <c r="J392" s="1">
+        <v>0</v>
       </c>
       <c r="K392" s="1">
         <v>1</v>
@@ -18072,8 +18072,8 @@
       <c r="E393" s="1">
         <v>4</v>
       </c>
-      <c r="F393" s="1" t="s">
-        <v>17</v>
+      <c r="F393" s="1">
+        <v>0</v>
       </c>
       <c r="G393" s="1">
         <v>1</v>
@@ -18084,8 +18084,8 @@
       <c r="I393" s="1">
         <v>4</v>
       </c>
-      <c r="J393" s="1" t="s">
-        <v>17</v>
+      <c r="J393" s="1">
+        <v>0</v>
       </c>
       <c r="K393" s="1">
         <v>1</v>
@@ -18116,8 +18116,8 @@
       <c r="E394" s="1">
         <v>4</v>
       </c>
-      <c r="F394" s="1" t="s">
-        <v>17</v>
+      <c r="F394" s="1">
+        <v>0</v>
       </c>
       <c r="G394" s="1">
         <v>1</v>
@@ -18128,8 +18128,8 @@
       <c r="I394" s="1">
         <v>4</v>
       </c>
-      <c r="J394" s="1" t="s">
-        <v>17</v>
+      <c r="J394" s="1">
+        <v>0</v>
       </c>
       <c r="K394" s="1">
         <v>1</v>
@@ -18160,8 +18160,8 @@
       <c r="E395" s="1">
         <v>4</v>
       </c>
-      <c r="F395" s="1" t="s">
-        <v>17</v>
+      <c r="F395" s="1">
+        <v>0</v>
       </c>
       <c r="G395" s="1">
         <v>1</v>
@@ -18172,8 +18172,8 @@
       <c r="I395" s="1">
         <v>4</v>
       </c>
-      <c r="J395" s="1" t="s">
-        <v>17</v>
+      <c r="J395" s="1">
+        <v>0</v>
       </c>
       <c r="K395" s="1">
         <v>1</v>
@@ -18204,8 +18204,8 @@
       <c r="E396" s="1">
         <v>4</v>
       </c>
-      <c r="F396" s="1" t="s">
-        <v>17</v>
+      <c r="F396" s="1">
+        <v>0</v>
       </c>
       <c r="G396" s="1">
         <v>1</v>
@@ -18216,8 +18216,8 @@
       <c r="I396" s="1">
         <v>4</v>
       </c>
-      <c r="J396" s="1" t="s">
-        <v>17</v>
+      <c r="J396" s="1">
+        <v>0</v>
       </c>
       <c r="K396" s="1">
         <v>1</v>
@@ -18248,8 +18248,8 @@
       <c r="E397" s="1">
         <v>4</v>
       </c>
-      <c r="F397" s="1" t="s">
-        <v>17</v>
+      <c r="F397" s="1">
+        <v>0</v>
       </c>
       <c r="G397" s="1">
         <v>1</v>
@@ -18260,8 +18260,8 @@
       <c r="I397" s="1">
         <v>4</v>
       </c>
-      <c r="J397" s="1" t="s">
-        <v>17</v>
+      <c r="J397" s="1">
+        <v>0</v>
       </c>
       <c r="K397" s="1">
         <v>1</v>
@@ -18292,8 +18292,8 @@
       <c r="E398" s="1">
         <v>4</v>
       </c>
-      <c r="F398" s="1" t="s">
-        <v>17</v>
+      <c r="F398" s="1">
+        <v>0</v>
       </c>
       <c r="G398" s="1">
         <v>1</v>
@@ -18304,8 +18304,8 @@
       <c r="I398" s="1">
         <v>4</v>
       </c>
-      <c r="J398" s="1" t="s">
-        <v>17</v>
+      <c r="J398" s="1">
+        <v>0</v>
       </c>
       <c r="K398" s="1">
         <v>1</v>
@@ -18336,8 +18336,8 @@
       <c r="E399" s="1">
         <v>4</v>
       </c>
-      <c r="F399" s="1" t="s">
-        <v>17</v>
+      <c r="F399" s="1">
+        <v>0</v>
       </c>
       <c r="G399" s="1">
         <v>1</v>
@@ -18348,8 +18348,8 @@
       <c r="I399" s="1">
         <v>4</v>
       </c>
-      <c r="J399" s="1" t="s">
-        <v>17</v>
+      <c r="J399" s="1">
+        <v>0</v>
       </c>
       <c r="K399" s="1">
         <v>1</v>
@@ -18380,8 +18380,8 @@
       <c r="E400" s="1">
         <v>4</v>
       </c>
-      <c r="F400" s="1" t="s">
-        <v>17</v>
+      <c r="F400" s="1">
+        <v>0</v>
       </c>
       <c r="G400" s="1">
         <v>1</v>
@@ -18392,8 +18392,8 @@
       <c r="I400" s="1">
         <v>4</v>
       </c>
-      <c r="J400" s="1" t="s">
-        <v>17</v>
+      <c r="J400" s="1">
+        <v>0</v>
       </c>
       <c r="K400" s="1">
         <v>1</v>
@@ -18424,8 +18424,8 @@
       <c r="E401" s="1">
         <v>4</v>
       </c>
-      <c r="F401" s="1" t="s">
-        <v>17</v>
+      <c r="F401" s="1">
+        <v>0</v>
       </c>
       <c r="G401" s="1">
         <v>1</v>
@@ -18436,8 +18436,8 @@
       <c r="I401" s="1">
         <v>4</v>
       </c>
-      <c r="J401" s="1" t="s">
-        <v>17</v>
+      <c r="J401" s="1">
+        <v>0</v>
       </c>
       <c r="K401" s="1">
         <v>1</v>
@@ -18468,8 +18468,8 @@
       <c r="E402" s="1">
         <v>4</v>
       </c>
-      <c r="F402" s="1" t="s">
-        <v>17</v>
+      <c r="F402" s="1">
+        <v>0</v>
       </c>
       <c r="G402" s="1">
         <v>1</v>
@@ -18480,8 +18480,8 @@
       <c r="I402" s="1">
         <v>4</v>
       </c>
-      <c r="J402" s="1" t="s">
-        <v>17</v>
+      <c r="J402" s="1">
+        <v>0</v>
       </c>
       <c r="K402" s="1">
         <v>1</v>
@@ -18512,8 +18512,8 @@
       <c r="E403" s="1">
         <v>4</v>
       </c>
-      <c r="F403" s="1" t="s">
-        <v>17</v>
+      <c r="F403" s="1">
+        <v>0</v>
       </c>
       <c r="G403" s="1">
         <v>1</v>
@@ -18524,8 +18524,8 @@
       <c r="I403" s="1">
         <v>4</v>
       </c>
-      <c r="J403" s="1" t="s">
-        <v>17</v>
+      <c r="J403" s="1">
+        <v>0</v>
       </c>
       <c r="K403" s="1">
         <v>1</v>
@@ -18556,8 +18556,8 @@
       <c r="E404" s="1">
         <v>4</v>
       </c>
-      <c r="F404" s="1" t="s">
-        <v>17</v>
+      <c r="F404" s="1">
+        <v>0</v>
       </c>
       <c r="G404" s="1">
         <v>1</v>
@@ -18568,8 +18568,8 @@
       <c r="I404" s="1">
         <v>4</v>
       </c>
-      <c r="J404" s="1" t="s">
-        <v>17</v>
+      <c r="J404" s="1">
+        <v>0</v>
       </c>
       <c r="K404" s="1">
         <v>1</v>
@@ -18600,8 +18600,8 @@
       <c r="E405" s="1">
         <v>4</v>
       </c>
-      <c r="F405" s="1" t="s">
-        <v>17</v>
+      <c r="F405" s="1">
+        <v>0</v>
       </c>
       <c r="G405" s="1">
         <v>1</v>
@@ -18612,8 +18612,8 @@
       <c r="I405" s="1">
         <v>4</v>
       </c>
-      <c r="J405" s="1" t="s">
-        <v>17</v>
+      <c r="J405" s="1">
+        <v>0</v>
       </c>
       <c r="K405" s="1">
         <v>1</v>
@@ -18644,8 +18644,8 @@
       <c r="E406" s="1">
         <v>4</v>
       </c>
-      <c r="F406" s="1" t="s">
-        <v>17</v>
+      <c r="F406" s="1">
+        <v>0</v>
       </c>
       <c r="G406" s="1">
         <v>1</v>
@@ -18656,8 +18656,8 @@
       <c r="I406" s="1">
         <v>4</v>
       </c>
-      <c r="J406" s="1" t="s">
-        <v>17</v>
+      <c r="J406" s="1">
+        <v>0</v>
       </c>
       <c r="K406" s="1">
         <v>1</v>
@@ -18688,8 +18688,8 @@
       <c r="E407" s="1">
         <v>4</v>
       </c>
-      <c r="F407" s="1" t="s">
-        <v>17</v>
+      <c r="F407" s="1">
+        <v>0</v>
       </c>
       <c r="G407" s="1">
         <v>1</v>
@@ -18700,8 +18700,8 @@
       <c r="I407" s="1">
         <v>4</v>
       </c>
-      <c r="J407" s="1" t="s">
-        <v>17</v>
+      <c r="J407" s="1">
+        <v>0</v>
       </c>
       <c r="K407" s="1">
         <v>1</v>
@@ -18732,8 +18732,8 @@
       <c r="E408" s="1">
         <v>4</v>
       </c>
-      <c r="F408" s="1" t="s">
-        <v>17</v>
+      <c r="F408" s="1">
+        <v>0</v>
       </c>
       <c r="G408" s="1">
         <v>1</v>
@@ -18744,8 +18744,8 @@
       <c r="I408" s="1">
         <v>4</v>
       </c>
-      <c r="J408" s="1" t="s">
-        <v>17</v>
+      <c r="J408" s="1">
+        <v>0</v>
       </c>
       <c r="K408" s="1">
         <v>1</v>
@@ -18776,8 +18776,8 @@
       <c r="E409" s="1">
         <v>4</v>
       </c>
-      <c r="F409" s="1" t="s">
-        <v>17</v>
+      <c r="F409" s="1">
+        <v>0</v>
       </c>
       <c r="G409" s="1">
         <v>1</v>
@@ -18788,8 +18788,8 @@
       <c r="I409" s="1">
         <v>4</v>
       </c>
-      <c r="J409" s="1" t="s">
-        <v>17</v>
+      <c r="J409" s="1">
+        <v>0</v>
       </c>
       <c r="K409" s="1">
         <v>1</v>
@@ -18820,8 +18820,8 @@
       <c r="E410" s="1">
         <v>4</v>
       </c>
-      <c r="F410" s="1" t="s">
-        <v>17</v>
+      <c r="F410" s="1">
+        <v>0</v>
       </c>
       <c r="G410" s="1">
         <v>1</v>
@@ -18832,8 +18832,8 @@
       <c r="I410" s="1">
         <v>4</v>
       </c>
-      <c r="J410" s="1" t="s">
-        <v>17</v>
+      <c r="J410" s="1">
+        <v>0</v>
       </c>
       <c r="K410" s="1">
         <v>1</v>
@@ -18864,8 +18864,8 @@
       <c r="E411" s="1">
         <v>4</v>
       </c>
-      <c r="F411" s="1" t="s">
-        <v>17</v>
+      <c r="F411" s="1">
+        <v>0</v>
       </c>
       <c r="G411" s="1">
         <v>1</v>
@@ -18876,8 +18876,8 @@
       <c r="I411" s="1">
         <v>4</v>
       </c>
-      <c r="J411" s="1" t="s">
-        <v>17</v>
+      <c r="J411" s="1">
+        <v>0</v>
       </c>
       <c r="K411" s="1">
         <v>1</v>
@@ -18908,8 +18908,8 @@
       <c r="E412" s="1">
         <v>4</v>
       </c>
-      <c r="F412" s="1" t="s">
-        <v>17</v>
+      <c r="F412" s="1">
+        <v>0</v>
       </c>
       <c r="G412" s="1">
         <v>1</v>
@@ -18920,8 +18920,8 @@
       <c r="I412" s="1">
         <v>4</v>
       </c>
-      <c r="J412" s="1" t="s">
-        <v>17</v>
+      <c r="J412" s="1">
+        <v>0</v>
       </c>
       <c r="K412" s="1">
         <v>1</v>
@@ -18952,8 +18952,8 @@
       <c r="E413" s="1">
         <v>4</v>
       </c>
-      <c r="F413" s="1" t="s">
-        <v>17</v>
+      <c r="F413" s="1">
+        <v>0</v>
       </c>
       <c r="G413" s="1">
         <v>1</v>
@@ -18964,8 +18964,8 @@
       <c r="I413" s="1">
         <v>4</v>
       </c>
-      <c r="J413" s="1" t="s">
-        <v>17</v>
+      <c r="J413" s="1">
+        <v>0</v>
       </c>
       <c r="K413" s="1">
         <v>1</v>
@@ -18996,8 +18996,8 @@
       <c r="E414" s="1">
         <v>4</v>
       </c>
-      <c r="F414" s="1" t="s">
-        <v>17</v>
+      <c r="F414" s="1">
+        <v>0</v>
       </c>
       <c r="G414" s="1">
         <v>1</v>
@@ -19008,8 +19008,8 @@
       <c r="I414" s="1">
         <v>4</v>
       </c>
-      <c r="J414" s="1" t="s">
-        <v>17</v>
+      <c r="J414" s="1">
+        <v>0</v>
       </c>
       <c r="K414" s="1">
         <v>1</v>
@@ -19040,8 +19040,8 @@
       <c r="E415" s="1">
         <v>4</v>
       </c>
-      <c r="F415" s="1" t="s">
-        <v>17</v>
+      <c r="F415" s="1">
+        <v>0</v>
       </c>
       <c r="G415" s="1">
         <v>1</v>
@@ -19052,8 +19052,8 @@
       <c r="I415" s="1">
         <v>4</v>
       </c>
-      <c r="J415" s="1" t="s">
-        <v>17</v>
+      <c r="J415" s="1">
+        <v>0</v>
       </c>
       <c r="K415" s="1">
         <v>1</v>
@@ -19084,8 +19084,8 @@
       <c r="E416" s="1">
         <v>4</v>
       </c>
-      <c r="F416" s="1" t="s">
-        <v>17</v>
+      <c r="F416" s="1">
+        <v>0</v>
       </c>
       <c r="G416" s="1">
         <v>1</v>
@@ -19096,8 +19096,8 @@
       <c r="I416" s="1">
         <v>4</v>
       </c>
-      <c r="J416" s="1" t="s">
-        <v>17</v>
+      <c r="J416" s="1">
+        <v>0</v>
       </c>
       <c r="K416" s="1">
         <v>1</v>
@@ -19128,8 +19128,8 @@
       <c r="E417" s="1">
         <v>4</v>
       </c>
-      <c r="F417" s="1" t="s">
-        <v>17</v>
+      <c r="F417" s="1">
+        <v>0</v>
       </c>
       <c r="G417" s="1">
         <v>1</v>
@@ -19140,8 +19140,8 @@
       <c r="I417" s="1">
         <v>4</v>
       </c>
-      <c r="J417" s="1" t="s">
-        <v>17</v>
+      <c r="J417" s="1">
+        <v>0</v>
       </c>
       <c r="K417" s="1">
         <v>1</v>
@@ -19172,8 +19172,8 @@
       <c r="E418" s="1">
         <v>4</v>
       </c>
-      <c r="F418" s="1" t="s">
-        <v>17</v>
+      <c r="F418" s="1">
+        <v>0</v>
       </c>
       <c r="G418" s="1">
         <v>1</v>
@@ -19184,8 +19184,8 @@
       <c r="I418" s="1">
         <v>4</v>
       </c>
-      <c r="J418" s="1" t="s">
-        <v>17</v>
+      <c r="J418" s="1">
+        <v>0</v>
       </c>
       <c r="K418" s="1">
         <v>1</v>
@@ -19216,8 +19216,8 @@
       <c r="E419" s="1">
         <v>4</v>
       </c>
-      <c r="F419" s="1" t="s">
-        <v>17</v>
+      <c r="F419" s="1">
+        <v>0</v>
       </c>
       <c r="G419" s="1">
         <v>1</v>
@@ -19228,8 +19228,8 @@
       <c r="I419" s="1">
         <v>4</v>
       </c>
-      <c r="J419" s="1" t="s">
-        <v>17</v>
+      <c r="J419" s="1">
+        <v>0</v>
       </c>
       <c r="K419" s="1">
         <v>1</v>
@@ -19260,8 +19260,8 @@
       <c r="E420" s="1">
         <v>4</v>
       </c>
-      <c r="F420" s="1" t="s">
-        <v>17</v>
+      <c r="F420" s="1">
+        <v>0</v>
       </c>
       <c r="G420" s="1">
         <v>1</v>
@@ -19272,8 +19272,8 @@
       <c r="I420" s="1">
         <v>4</v>
       </c>
-      <c r="J420" s="1" t="s">
-        <v>17</v>
+      <c r="J420" s="1">
+        <v>0</v>
       </c>
       <c r="K420" s="1">
         <v>1</v>
@@ -19304,8 +19304,8 @@
       <c r="E421" s="1">
         <v>4</v>
       </c>
-      <c r="F421" s="1" t="s">
-        <v>17</v>
+      <c r="F421" s="1">
+        <v>0</v>
       </c>
       <c r="G421" s="1">
         <v>1</v>
@@ -19316,8 +19316,8 @@
       <c r="I421" s="1">
         <v>4</v>
       </c>
-      <c r="J421" s="1" t="s">
-        <v>17</v>
+      <c r="J421" s="1">
+        <v>0</v>
       </c>
       <c r="K421" s="1">
         <v>1</v>
@@ -19348,8 +19348,8 @@
       <c r="E422" s="1">
         <v>4</v>
       </c>
-      <c r="F422" s="1" t="s">
-        <v>17</v>
+      <c r="F422" s="1">
+        <v>0</v>
       </c>
       <c r="G422" s="1">
         <v>1</v>
@@ -19360,8 +19360,8 @@
       <c r="I422" s="1">
         <v>4</v>
       </c>
-      <c r="J422" s="1" t="s">
-        <v>17</v>
+      <c r="J422" s="1">
+        <v>0</v>
       </c>
       <c r="K422" s="1">
         <v>1</v>
@@ -19392,8 +19392,8 @@
       <c r="E423" s="1">
         <v>4</v>
       </c>
-      <c r="F423" s="1" t="s">
-        <v>17</v>
+      <c r="F423" s="1">
+        <v>0</v>
       </c>
       <c r="G423" s="1">
         <v>1</v>
@@ -19404,8 +19404,8 @@
       <c r="I423" s="1">
         <v>4</v>
       </c>
-      <c r="J423" s="1" t="s">
-        <v>17</v>
+      <c r="J423" s="1">
+        <v>0</v>
       </c>
       <c r="K423" s="1">
         <v>1</v>
@@ -19436,8 +19436,8 @@
       <c r="E424" s="1">
         <v>4</v>
       </c>
-      <c r="F424" s="1" t="s">
-        <v>17</v>
+      <c r="F424" s="1">
+        <v>0</v>
       </c>
       <c r="G424" s="1">
         <v>1</v>
@@ -19448,8 +19448,8 @@
       <c r="I424" s="1">
         <v>4</v>
       </c>
-      <c r="J424" s="1" t="s">
-        <v>17</v>
+      <c r="J424" s="1">
+        <v>0</v>
       </c>
       <c r="K424" s="1">
         <v>1</v>
@@ -19480,8 +19480,8 @@
       <c r="E425" s="1">
         <v>4</v>
       </c>
-      <c r="F425" s="1" t="s">
-        <v>17</v>
+      <c r="F425" s="1">
+        <v>0</v>
       </c>
       <c r="G425" s="1">
         <v>1</v>
@@ -19492,8 +19492,8 @@
       <c r="I425" s="1">
         <v>4</v>
       </c>
-      <c r="J425" s="1" t="s">
-        <v>17</v>
+      <c r="J425" s="1">
+        <v>0</v>
       </c>
       <c r="K425" s="1">
         <v>1</v>
@@ -19524,8 +19524,8 @@
       <c r="E426" s="1">
         <v>4</v>
       </c>
-      <c r="F426" s="1" t="s">
-        <v>17</v>
+      <c r="F426" s="1">
+        <v>0</v>
       </c>
       <c r="G426" s="1">
         <v>1</v>
@@ -19536,8 +19536,8 @@
       <c r="I426" s="1">
         <v>4</v>
       </c>
-      <c r="J426" s="1" t="s">
-        <v>17</v>
+      <c r="J426" s="1">
+        <v>0</v>
       </c>
       <c r="K426" s="1">
         <v>1</v>
@@ -19568,8 +19568,8 @@
       <c r="E427" s="1">
         <v>4</v>
       </c>
-      <c r="F427" s="1" t="s">
-        <v>17</v>
+      <c r="F427" s="1">
+        <v>0</v>
       </c>
       <c r="G427" s="1">
         <v>1</v>
@@ -19580,8 +19580,8 @@
       <c r="I427" s="1">
         <v>4</v>
       </c>
-      <c r="J427" s="1" t="s">
-        <v>17</v>
+      <c r="J427" s="1">
+        <v>0</v>
       </c>
       <c r="K427" s="1">
         <v>1</v>
@@ -19612,8 +19612,8 @@
       <c r="E428" s="1">
         <v>4</v>
       </c>
-      <c r="F428" s="1" t="s">
-        <v>17</v>
+      <c r="F428" s="1">
+        <v>0</v>
       </c>
       <c r="G428" s="1">
         <v>1</v>
@@ -19624,8 +19624,8 @@
       <c r="I428" s="1">
         <v>4</v>
       </c>
-      <c r="J428" s="1" t="s">
-        <v>17</v>
+      <c r="J428" s="1">
+        <v>0</v>
       </c>
       <c r="K428" s="1">
         <v>1</v>
@@ -19656,8 +19656,8 @@
       <c r="E429" s="1">
         <v>4</v>
       </c>
-      <c r="F429" s="1" t="s">
-        <v>17</v>
+      <c r="F429" s="1">
+        <v>0</v>
       </c>
       <c r="G429" s="1">
         <v>1</v>
@@ -19668,8 +19668,8 @@
       <c r="I429" s="1">
         <v>4</v>
       </c>
-      <c r="J429" s="1" t="s">
-        <v>17</v>
+      <c r="J429" s="1">
+        <v>0</v>
       </c>
       <c r="K429" s="1">
         <v>1</v>
@@ -19700,8 +19700,8 @@
       <c r="E430" s="1">
         <v>4</v>
       </c>
-      <c r="F430" s="1" t="s">
-        <v>17</v>
+      <c r="F430" s="1">
+        <v>0</v>
       </c>
       <c r="G430" s="1">
         <v>1</v>
@@ -19712,8 +19712,8 @@
       <c r="I430" s="1">
         <v>4</v>
       </c>
-      <c r="J430" s="1" t="s">
-        <v>17</v>
+      <c r="J430" s="1">
+        <v>0</v>
       </c>
       <c r="K430" s="1">
         <v>1</v>
@@ -19744,8 +19744,8 @@
       <c r="E431" s="1">
         <v>4</v>
       </c>
-      <c r="F431" s="1" t="s">
-        <v>17</v>
+      <c r="F431" s="1">
+        <v>0</v>
       </c>
       <c r="G431" s="1">
         <v>1</v>
@@ -19756,8 +19756,8 @@
       <c r="I431" s="1">
         <v>4</v>
       </c>
-      <c r="J431" s="1" t="s">
-        <v>17</v>
+      <c r="J431" s="1">
+        <v>0</v>
       </c>
       <c r="K431" s="1">
         <v>1</v>
@@ -19788,8 +19788,8 @@
       <c r="E432" s="1">
         <v>4</v>
       </c>
-      <c r="F432" s="1" t="s">
-        <v>17</v>
+      <c r="F432" s="1">
+        <v>0</v>
       </c>
       <c r="G432" s="1">
         <v>1</v>
@@ -19800,8 +19800,8 @@
       <c r="I432" s="1">
         <v>4</v>
       </c>
-      <c r="J432" s="1" t="s">
-        <v>17</v>
+      <c r="J432" s="1">
+        <v>0</v>
       </c>
       <c r="K432" s="1">
         <v>1</v>
@@ -19832,8 +19832,8 @@
       <c r="E433" s="1">
         <v>4</v>
       </c>
-      <c r="F433" s="1" t="s">
-        <v>17</v>
+      <c r="F433" s="1">
+        <v>0</v>
       </c>
       <c r="G433" s="1">
         <v>1</v>
@@ -19844,8 +19844,8 @@
       <c r="I433" s="1">
         <v>4</v>
       </c>
-      <c r="J433" s="1" t="s">
-        <v>17</v>
+      <c r="J433" s="1">
+        <v>0</v>
       </c>
       <c r="K433" s="1">
         <v>1</v>
@@ -19876,8 +19876,8 @@
       <c r="E434" s="1">
         <v>4</v>
       </c>
-      <c r="F434" s="1" t="s">
-        <v>17</v>
+      <c r="F434" s="1">
+        <v>0</v>
       </c>
       <c r="G434" s="1">
         <v>1</v>
@@ -19888,8 +19888,8 @@
       <c r="I434" s="1">
         <v>4</v>
       </c>
-      <c r="J434" s="1" t="s">
-        <v>17</v>
+      <c r="J434" s="1">
+        <v>0</v>
       </c>
       <c r="K434" s="1">
         <v>1</v>
@@ -19920,8 +19920,8 @@
       <c r="E435" s="1">
         <v>4</v>
       </c>
-      <c r="F435" s="1" t="s">
-        <v>17</v>
+      <c r="F435" s="1">
+        <v>0</v>
       </c>
       <c r="G435" s="1">
         <v>1</v>
@@ -19932,8 +19932,8 @@
       <c r="I435" s="1">
         <v>4</v>
       </c>
-      <c r="J435" s="1" t="s">
-        <v>17</v>
+      <c r="J435" s="1">
+        <v>0</v>
       </c>
       <c r="K435" s="1">
         <v>1</v>
@@ -19964,8 +19964,8 @@
       <c r="E436" s="1">
         <v>4</v>
       </c>
-      <c r="F436" s="1" t="s">
-        <v>17</v>
+      <c r="F436" s="1">
+        <v>0</v>
       </c>
       <c r="G436" s="1">
         <v>1</v>
@@ -19976,8 +19976,8 @@
       <c r="I436" s="1">
         <v>4</v>
       </c>
-      <c r="J436" s="1" t="s">
-        <v>17</v>
+      <c r="J436" s="1">
+        <v>0</v>
       </c>
       <c r="K436" s="1">
         <v>1</v>
@@ -20008,8 +20008,8 @@
       <c r="E437" s="1">
         <v>4</v>
       </c>
-      <c r="F437" s="1" t="s">
-        <v>17</v>
+      <c r="F437" s="1">
+        <v>0</v>
       </c>
       <c r="G437" s="1">
         <v>1</v>
@@ -20020,8 +20020,8 @@
       <c r="I437" s="1">
         <v>4</v>
       </c>
-      <c r="J437" s="1" t="s">
-        <v>17</v>
+      <c r="J437" s="1">
+        <v>0</v>
       </c>
       <c r="K437" s="1">
         <v>1</v>
@@ -20052,8 +20052,8 @@
       <c r="E438" s="1">
         <v>4</v>
       </c>
-      <c r="F438" s="1" t="s">
-        <v>17</v>
+      <c r="F438" s="1">
+        <v>0</v>
       </c>
       <c r="G438" s="1">
         <v>1</v>
@@ -20064,8 +20064,8 @@
       <c r="I438" s="1">
         <v>4</v>
       </c>
-      <c r="J438" s="1" t="s">
-        <v>17</v>
+      <c r="J438" s="1">
+        <v>0</v>
       </c>
       <c r="K438" s="1">
         <v>1</v>
@@ -20096,8 +20096,8 @@
       <c r="E439" s="1">
         <v>4</v>
       </c>
-      <c r="F439" s="1" t="s">
-        <v>17</v>
+      <c r="F439" s="1">
+        <v>0</v>
       </c>
       <c r="G439" s="1">
         <v>1</v>
@@ -20108,8 +20108,8 @@
       <c r="I439" s="1">
         <v>4</v>
       </c>
-      <c r="J439" s="1" t="s">
-        <v>17</v>
+      <c r="J439" s="1">
+        <v>0</v>
       </c>
       <c r="K439" s="1">
         <v>1</v>
@@ -20140,8 +20140,8 @@
       <c r="E440" s="1">
         <v>4</v>
       </c>
-      <c r="F440" s="1" t="s">
-        <v>17</v>
+      <c r="F440" s="1">
+        <v>0</v>
       </c>
       <c r="G440" s="1">
         <v>1</v>
@@ -20152,8 +20152,8 @@
       <c r="I440" s="1">
         <v>4</v>
       </c>
-      <c r="J440" s="1" t="s">
-        <v>17</v>
+      <c r="J440" s="1">
+        <v>0</v>
       </c>
       <c r="K440" s="1">
         <v>1</v>
@@ -20184,8 +20184,8 @@
       <c r="E441" s="1">
         <v>4</v>
       </c>
-      <c r="F441" s="1" t="s">
-        <v>17</v>
+      <c r="F441" s="1">
+        <v>0</v>
       </c>
       <c r="G441" s="1">
         <v>1</v>
@@ -20196,8 +20196,8 @@
       <c r="I441" s="1">
         <v>4</v>
       </c>
-      <c r="J441" s="1" t="s">
-        <v>17</v>
+      <c r="J441" s="1">
+        <v>0</v>
       </c>
       <c r="K441" s="1">
         <v>1</v>
@@ -20228,8 +20228,8 @@
       <c r="E442" s="1">
         <v>4</v>
       </c>
-      <c r="F442" s="1" t="s">
-        <v>17</v>
+      <c r="F442" s="1">
+        <v>0</v>
       </c>
       <c r="G442" s="1">
         <v>1</v>
@@ -20240,8 +20240,8 @@
       <c r="I442" s="1">
         <v>4</v>
       </c>
-      <c r="J442" s="1" t="s">
-        <v>17</v>
+      <c r="J442" s="1">
+        <v>0</v>
       </c>
       <c r="K442" s="1">
         <v>1</v>
@@ -20272,8 +20272,8 @@
       <c r="E443" s="1">
         <v>4</v>
       </c>
-      <c r="F443" s="1" t="s">
-        <v>17</v>
+      <c r="F443" s="1">
+        <v>0</v>
       </c>
       <c r="G443" s="1">
         <v>1</v>
@@ -20284,8 +20284,8 @@
       <c r="I443" s="1">
         <v>4</v>
       </c>
-      <c r="J443" s="1" t="s">
-        <v>17</v>
+      <c r="J443" s="1">
+        <v>0</v>
       </c>
       <c r="K443" s="1">
         <v>1</v>
@@ -20316,8 +20316,8 @@
       <c r="E444" s="1">
         <v>4</v>
       </c>
-      <c r="F444" s="1" t="s">
-        <v>17</v>
+      <c r="F444" s="1">
+        <v>0</v>
       </c>
       <c r="G444" s="1">
         <v>1</v>
@@ -20328,8 +20328,8 @@
       <c r="I444" s="1">
         <v>4</v>
       </c>
-      <c r="J444" s="1" t="s">
-        <v>17</v>
+      <c r="J444" s="1">
+        <v>0</v>
       </c>
       <c r="K444" s="1">
         <v>1</v>
@@ -20360,8 +20360,8 @@
       <c r="E445" s="1">
         <v>4</v>
       </c>
-      <c r="F445" s="1" t="s">
-        <v>17</v>
+      <c r="F445" s="1">
+        <v>0</v>
       </c>
       <c r="G445" s="1">
         <v>1</v>
@@ -20372,8 +20372,8 @@
       <c r="I445" s="1">
         <v>4</v>
       </c>
-      <c r="J445" s="1" t="s">
-        <v>17</v>
+      <c r="J445" s="1">
+        <v>0</v>
       </c>
       <c r="K445" s="1">
         <v>1</v>
@@ -20404,8 +20404,8 @@
       <c r="E446" s="1">
         <v>4</v>
       </c>
-      <c r="F446" s="1" t="s">
-        <v>17</v>
+      <c r="F446" s="1">
+        <v>0</v>
       </c>
       <c r="G446" s="1">
         <v>1</v>
@@ -20416,8 +20416,8 @@
       <c r="I446" s="1">
         <v>4</v>
       </c>
-      <c r="J446" s="1" t="s">
-        <v>17</v>
+      <c r="J446" s="1">
+        <v>0</v>
       </c>
       <c r="K446" s="1">
         <v>1</v>
@@ -20448,8 +20448,8 @@
       <c r="E447" s="1">
         <v>4</v>
       </c>
-      <c r="F447" s="1" t="s">
-        <v>17</v>
+      <c r="F447" s="1">
+        <v>0</v>
       </c>
       <c r="G447" s="1">
         <v>1</v>
@@ -20460,8 +20460,8 @@
       <c r="I447" s="1">
         <v>4</v>
       </c>
-      <c r="J447" s="1" t="s">
-        <v>17</v>
+      <c r="J447" s="1">
+        <v>0</v>
       </c>
       <c r="K447" s="1">
         <v>1</v>
@@ -20492,8 +20492,8 @@
       <c r="E448" s="1">
         <v>4</v>
       </c>
-      <c r="F448" s="1" t="s">
-        <v>17</v>
+      <c r="F448" s="1">
+        <v>0</v>
       </c>
       <c r="G448" s="1">
         <v>1</v>
@@ -20504,8 +20504,8 @@
       <c r="I448" s="1">
         <v>4</v>
       </c>
-      <c r="J448" s="1" t="s">
-        <v>17</v>
+      <c r="J448" s="1">
+        <v>0</v>
       </c>
       <c r="K448" s="1">
         <v>1</v>
@@ -20536,8 +20536,8 @@
       <c r="E449" s="1">
         <v>4</v>
       </c>
-      <c r="F449" s="1" t="s">
-        <v>17</v>
+      <c r="F449" s="1">
+        <v>0</v>
       </c>
       <c r="G449" s="1">
         <v>1</v>
@@ -20548,8 +20548,8 @@
       <c r="I449" s="1">
         <v>4</v>
       </c>
-      <c r="J449" s="1" t="s">
-        <v>17</v>
+      <c r="J449" s="1">
+        <v>0</v>
       </c>
       <c r="K449" s="1">
         <v>1</v>
@@ -20580,8 +20580,8 @@
       <c r="E450" s="1">
         <v>4</v>
       </c>
-      <c r="F450" s="1" t="s">
-        <v>17</v>
+      <c r="F450" s="1">
+        <v>0</v>
       </c>
       <c r="G450" s="1">
         <v>1</v>
@@ -20592,8 +20592,8 @@
       <c r="I450" s="1">
         <v>4</v>
       </c>
-      <c r="J450" s="1" t="s">
-        <v>17</v>
+      <c r="J450" s="1">
+        <v>0</v>
       </c>
       <c r="K450" s="1">
         <v>1</v>
@@ -20624,8 +20624,8 @@
       <c r="E451" s="1">
         <v>4</v>
       </c>
-      <c r="F451" s="1" t="s">
-        <v>17</v>
+      <c r="F451" s="1">
+        <v>0</v>
       </c>
       <c r="G451" s="1">
         <v>1</v>
@@ -20636,8 +20636,8 @@
       <c r="I451" s="1">
         <v>4</v>
       </c>
-      <c r="J451" s="1" t="s">
-        <v>17</v>
+      <c r="J451" s="1">
+        <v>0</v>
       </c>
       <c r="K451" s="1">
         <v>1</v>
@@ -20668,8 +20668,8 @@
       <c r="E452" s="1">
         <v>4</v>
       </c>
-      <c r="F452" s="1" t="s">
-        <v>17</v>
+      <c r="F452" s="1">
+        <v>0</v>
       </c>
       <c r="G452" s="1">
         <v>1</v>
@@ -20680,8 +20680,8 @@
       <c r="I452" s="1">
         <v>4</v>
       </c>
-      <c r="J452" s="1" t="s">
-        <v>17</v>
+      <c r="J452" s="1">
+        <v>0</v>
       </c>
       <c r="K452" s="1">
         <v>1</v>
@@ -20712,8 +20712,8 @@
       <c r="E453" s="1">
         <v>4</v>
       </c>
-      <c r="F453" s="1" t="s">
-        <v>17</v>
+      <c r="F453" s="1">
+        <v>0</v>
       </c>
       <c r="G453" s="1">
         <v>1</v>
@@ -20724,8 +20724,8 @@
       <c r="I453" s="1">
         <v>4</v>
       </c>
-      <c r="J453" s="1" t="s">
-        <v>17</v>
+      <c r="J453" s="1">
+        <v>0</v>
       </c>
       <c r="K453" s="1">
         <v>1</v>
@@ -20756,8 +20756,8 @@
       <c r="E454" s="1">
         <v>4</v>
       </c>
-      <c r="F454" s="1" t="s">
-        <v>17</v>
+      <c r="F454" s="1">
+        <v>0</v>
       </c>
       <c r="G454" s="1">
         <v>1</v>
@@ -20768,8 +20768,8 @@
       <c r="I454" s="1">
         <v>4</v>
       </c>
-      <c r="J454" s="1" t="s">
-        <v>17</v>
+      <c r="J454" s="1">
+        <v>0</v>
       </c>
       <c r="K454" s="1">
         <v>1</v>
@@ -20800,8 +20800,8 @@
       <c r="E455" s="1">
         <v>4</v>
       </c>
-      <c r="F455" s="1" t="s">
-        <v>17</v>
+      <c r="F455" s="1">
+        <v>0</v>
       </c>
       <c r="G455" s="1">
         <v>1</v>
@@ -20812,8 +20812,8 @@
       <c r="I455" s="1">
         <v>4</v>
       </c>
-      <c r="J455" s="1" t="s">
-        <v>17</v>
+      <c r="J455" s="1">
+        <v>0</v>
       </c>
       <c r="K455" s="1">
         <v>1</v>
@@ -20844,8 +20844,8 @@
       <c r="E456" s="1">
         <v>4</v>
       </c>
-      <c r="F456" s="1" t="s">
-        <v>17</v>
+      <c r="F456" s="1">
+        <v>0</v>
       </c>
       <c r="G456" s="1">
         <v>1</v>
@@ -20856,8 +20856,8 @@
       <c r="I456" s="1">
         <v>4</v>
       </c>
-      <c r="J456" s="1" t="s">
-        <v>17</v>
+      <c r="J456" s="1">
+        <v>0</v>
       </c>
       <c r="K456" s="1">
         <v>1</v>
@@ -20888,8 +20888,8 @@
       <c r="E457" s="1">
         <v>4</v>
       </c>
-      <c r="F457" s="1" t="s">
-        <v>17</v>
+      <c r="F457" s="1">
+        <v>0</v>
       </c>
       <c r="G457" s="1">
         <v>1</v>
@@ -20900,8 +20900,8 @@
       <c r="I457" s="1">
         <v>4</v>
       </c>
-      <c r="J457" s="1" t="s">
-        <v>17</v>
+      <c r="J457" s="1">
+        <v>0</v>
       </c>
       <c r="K457" s="1">
         <v>1</v>
@@ -20932,8 +20932,8 @@
       <c r="E458" s="1">
         <v>4</v>
       </c>
-      <c r="F458" s="1" t="s">
-        <v>17</v>
+      <c r="F458" s="1">
+        <v>0</v>
       </c>
       <c r="G458" s="1">
         <v>1</v>
@@ -20944,8 +20944,8 @@
       <c r="I458" s="1">
         <v>4</v>
       </c>
-      <c r="J458" s="1" t="s">
-        <v>17</v>
+      <c r="J458" s="1">
+        <v>0</v>
       </c>
       <c r="K458" s="1">
         <v>1</v>
@@ -20976,8 +20976,8 @@
       <c r="E459" s="1">
         <v>4</v>
       </c>
-      <c r="F459" s="1" t="s">
-        <v>17</v>
+      <c r="F459" s="1">
+        <v>0</v>
       </c>
       <c r="G459" s="1">
         <v>1</v>
@@ -20988,8 +20988,8 @@
       <c r="I459" s="1">
         <v>4</v>
       </c>
-      <c r="J459" s="1" t="s">
-        <v>17</v>
+      <c r="J459" s="1">
+        <v>0</v>
       </c>
       <c r="K459" s="1">
         <v>1</v>
@@ -21020,8 +21020,8 @@
       <c r="E460" s="1">
         <v>4</v>
       </c>
-      <c r="F460" s="1" t="s">
-        <v>17</v>
+      <c r="F460" s="1">
+        <v>0</v>
       </c>
       <c r="G460" s="1">
         <v>1</v>
@@ -21032,8 +21032,8 @@
       <c r="I460" s="1">
         <v>4</v>
       </c>
-      <c r="J460" s="1" t="s">
-        <v>17</v>
+      <c r="J460" s="1">
+        <v>0</v>
       </c>
       <c r="K460" s="1">
         <v>1</v>
@@ -21064,8 +21064,8 @@
       <c r="E461" s="1">
         <v>4</v>
       </c>
-      <c r="F461" s="1" t="s">
-        <v>17</v>
+      <c r="F461" s="1">
+        <v>0</v>
       </c>
       <c r="G461" s="1">
         <v>1</v>
@@ -21076,8 +21076,8 @@
       <c r="I461" s="1">
         <v>4</v>
       </c>
-      <c r="J461" s="1" t="s">
-        <v>17</v>
+      <c r="J461" s="1">
+        <v>0</v>
       </c>
       <c r="K461" s="1">
         <v>1</v>
@@ -21108,8 +21108,8 @@
       <c r="E462" s="1">
         <v>4</v>
       </c>
-      <c r="F462" s="1" t="s">
-        <v>17</v>
+      <c r="F462" s="1">
+        <v>0</v>
       </c>
       <c r="G462" s="1">
         <v>1</v>
@@ -21120,8 +21120,8 @@
       <c r="I462" s="1">
         <v>4</v>
       </c>
-      <c r="J462" s="1" t="s">
-        <v>17</v>
+      <c r="J462" s="1">
+        <v>0</v>
       </c>
       <c r="K462" s="1">
         <v>1</v>
@@ -21152,8 +21152,8 @@
       <c r="E463" s="1">
         <v>4</v>
       </c>
-      <c r="F463" s="1" t="s">
-        <v>17</v>
+      <c r="F463" s="1">
+        <v>0</v>
       </c>
       <c r="G463" s="1">
         <v>1</v>
@@ -21164,8 +21164,8 @@
       <c r="I463" s="1">
         <v>4</v>
       </c>
-      <c r="J463" s="1" t="s">
-        <v>17</v>
+      <c r="J463" s="1">
+        <v>0</v>
       </c>
       <c r="K463" s="1">
         <v>1</v>
@@ -21196,8 +21196,8 @@
       <c r="E464" s="1">
         <v>4</v>
       </c>
-      <c r="F464" s="1" t="s">
-        <v>17</v>
+      <c r="F464" s="1">
+        <v>0</v>
       </c>
       <c r="G464" s="1">
         <v>1</v>
@@ -21208,8 +21208,8 @@
       <c r="I464" s="1">
         <v>4</v>
       </c>
-      <c r="J464" s="1" t="s">
-        <v>17</v>
+      <c r="J464" s="1">
+        <v>0</v>
       </c>
       <c r="K464" s="1">
         <v>1</v>
@@ -21240,8 +21240,8 @@
       <c r="E465" s="1">
         <v>4</v>
       </c>
-      <c r="F465" s="1" t="s">
-        <v>17</v>
+      <c r="F465" s="1">
+        <v>0</v>
       </c>
       <c r="G465" s="1">
         <v>1</v>
@@ -21252,8 +21252,8 @@
       <c r="I465" s="1">
         <v>4</v>
       </c>
-      <c r="J465" s="1" t="s">
-        <v>17</v>
+      <c r="J465" s="1">
+        <v>0</v>
       </c>
       <c r="K465" s="1">
         <v>1</v>
@@ -21284,8 +21284,8 @@
       <c r="E466" s="1">
         <v>4</v>
       </c>
-      <c r="F466" s="1" t="s">
-        <v>17</v>
+      <c r="F466" s="1">
+        <v>0</v>
       </c>
       <c r="G466" s="1">
         <v>1</v>
@@ -21296,8 +21296,8 @@
       <c r="I466" s="1">
         <v>4</v>
       </c>
-      <c r="J466" s="1" t="s">
-        <v>17</v>
+      <c r="J466" s="1">
+        <v>0</v>
       </c>
       <c r="K466" s="1">
         <v>1</v>
@@ -21328,8 +21328,8 @@
       <c r="E467" s="1">
         <v>4</v>
       </c>
-      <c r="F467" s="1" t="s">
-        <v>17</v>
+      <c r="F467" s="1">
+        <v>0</v>
       </c>
       <c r="G467" s="1">
         <v>1</v>
@@ -21340,8 +21340,8 @@
       <c r="I467" s="1">
         <v>4</v>
       </c>
-      <c r="J467" s="1" t="s">
-        <v>17</v>
+      <c r="J467" s="1">
+        <v>0</v>
       </c>
       <c r="K467" s="1">
         <v>1</v>
@@ -21372,8 +21372,8 @@
       <c r="E468" s="1">
         <v>4</v>
       </c>
-      <c r="F468" s="1" t="s">
-        <v>17</v>
+      <c r="F468" s="1">
+        <v>0</v>
       </c>
       <c r="G468" s="1">
         <v>1</v>
@@ -21384,8 +21384,8 @@
       <c r="I468" s="1">
         <v>4</v>
       </c>
-      <c r="J468" s="1" t="s">
-        <v>17</v>
+      <c r="J468" s="1">
+        <v>0</v>
       </c>
       <c r="K468" s="1">
         <v>1</v>
@@ -21416,8 +21416,8 @@
       <c r="E469" s="1">
         <v>4</v>
       </c>
-      <c r="F469" s="1" t="s">
-        <v>17</v>
+      <c r="F469" s="1">
+        <v>0</v>
       </c>
       <c r="G469" s="1">
         <v>1</v>
@@ -21428,8 +21428,8 @@
       <c r="I469" s="1">
         <v>4</v>
       </c>
-      <c r="J469" s="1" t="s">
-        <v>17</v>
+      <c r="J469" s="1">
+        <v>0</v>
       </c>
       <c r="K469" s="1">
         <v>1</v>
@@ -21460,8 +21460,8 @@
       <c r="E470" s="1">
         <v>4</v>
       </c>
-      <c r="F470" s="1" t="s">
-        <v>17</v>
+      <c r="F470" s="1">
+        <v>0</v>
       </c>
       <c r="G470" s="1">
         <v>1</v>
@@ -21472,8 +21472,8 @@
       <c r="I470" s="1">
         <v>4</v>
       </c>
-      <c r="J470" s="1" t="s">
-        <v>17</v>
+      <c r="J470" s="1">
+        <v>0</v>
       </c>
       <c r="K470" s="1">
         <v>1</v>
@@ -21504,8 +21504,8 @@
       <c r="E471" s="1">
         <v>4</v>
       </c>
-      <c r="F471" s="1" t="s">
-        <v>17</v>
+      <c r="F471" s="1">
+        <v>0</v>
       </c>
       <c r="G471" s="1">
         <v>1</v>
@@ -21516,8 +21516,8 @@
       <c r="I471" s="1">
         <v>4</v>
       </c>
-      <c r="J471" s="1" t="s">
-        <v>17</v>
+      <c r="J471" s="1">
+        <v>0</v>
       </c>
       <c r="K471" s="1">
         <v>1</v>
@@ -21548,8 +21548,8 @@
       <c r="E472" s="1">
         <v>4</v>
       </c>
-      <c r="F472" s="1" t="s">
-        <v>17</v>
+      <c r="F472" s="1">
+        <v>0</v>
       </c>
       <c r="G472" s="1">
         <v>1</v>
@@ -21560,8 +21560,8 @@
       <c r="I472" s="1">
         <v>4</v>
       </c>
-      <c r="J472" s="1" t="s">
-        <v>17</v>
+      <c r="J472" s="1">
+        <v>0</v>
       </c>
       <c r="K472" s="1">
         <v>1</v>
@@ -21592,8 +21592,8 @@
       <c r="E473" s="1">
         <v>4</v>
       </c>
-      <c r="F473" s="1" t="s">
-        <v>17</v>
+      <c r="F473" s="1">
+        <v>0</v>
       </c>
       <c r="G473" s="1">
         <v>1</v>
@@ -21604,8 +21604,8 @@
       <c r="I473" s="1">
         <v>4</v>
       </c>
-      <c r="J473" s="1" t="s">
-        <v>17</v>
+      <c r="J473" s="1">
+        <v>0</v>
       </c>
       <c r="K473" s="1">
         <v>1</v>
@@ -21636,8 +21636,8 @@
       <c r="E474" s="1">
         <v>4</v>
       </c>
-      <c r="F474" s="1" t="s">
-        <v>17</v>
+      <c r="F474" s="1">
+        <v>0</v>
       </c>
       <c r="G474" s="1">
         <v>1</v>
@@ -21648,8 +21648,8 @@
       <c r="I474" s="1">
         <v>4</v>
       </c>
-      <c r="J474" s="1" t="s">
-        <v>17</v>
+      <c r="J474" s="1">
+        <v>0</v>
       </c>
       <c r="K474" s="1">
         <v>1</v>
@@ -21680,8 +21680,8 @@
       <c r="E475" s="1">
         <v>4</v>
       </c>
-      <c r="F475" s="1" t="s">
-        <v>17</v>
+      <c r="F475" s="1">
+        <v>0</v>
       </c>
       <c r="G475" s="1">
         <v>1</v>
@@ -21692,8 +21692,8 @@
       <c r="I475" s="1">
         <v>4</v>
       </c>
-      <c r="J475" s="1" t="s">
-        <v>17</v>
+      <c r="J475" s="1">
+        <v>0</v>
       </c>
       <c r="K475" s="1">
         <v>1</v>
@@ -21724,8 +21724,8 @@
       <c r="E476" s="1">
         <v>4</v>
       </c>
-      <c r="F476" s="1" t="s">
-        <v>17</v>
+      <c r="F476" s="1">
+        <v>0</v>
       </c>
       <c r="G476" s="1">
         <v>1</v>
@@ -21736,8 +21736,8 @@
       <c r="I476" s="1">
         <v>4</v>
       </c>
-      <c r="J476" s="1" t="s">
-        <v>17</v>
+      <c r="J476" s="1">
+        <v>0</v>
       </c>
       <c r="K476" s="1">
         <v>1</v>
@@ -21768,8 +21768,8 @@
       <c r="E477" s="1">
         <v>4</v>
       </c>
-      <c r="F477" s="1" t="s">
-        <v>17</v>
+      <c r="F477" s="1">
+        <v>0</v>
       </c>
       <c r="G477" s="1">
         <v>1</v>
@@ -21780,8 +21780,8 @@
       <c r="I477" s="1">
         <v>4</v>
       </c>
-      <c r="J477" s="1" t="s">
-        <v>17</v>
+      <c r="J477" s="1">
+        <v>0</v>
       </c>
       <c r="K477" s="1">
         <v>1</v>
@@ -21812,8 +21812,8 @@
       <c r="E478" s="1">
         <v>4</v>
       </c>
-      <c r="F478" s="1" t="s">
-        <v>17</v>
+      <c r="F478" s="1">
+        <v>0</v>
       </c>
       <c r="G478" s="1">
         <v>1</v>
@@ -21824,8 +21824,8 @@
       <c r="I478" s="1">
         <v>4</v>
       </c>
-      <c r="J478" s="1" t="s">
-        <v>17</v>
+      <c r="J478" s="1">
+        <v>0</v>
       </c>
       <c r="K478" s="1">
         <v>1</v>
@@ -21856,8 +21856,8 @@
       <c r="E479" s="1">
         <v>4</v>
       </c>
-      <c r="F479" s="1" t="s">
-        <v>17</v>
+      <c r="F479" s="1">
+        <v>0</v>
       </c>
       <c r="G479" s="1">
         <v>1</v>
@@ -21868,8 +21868,8 @@
       <c r="I479" s="1">
         <v>4</v>
       </c>
-      <c r="J479" s="1" t="s">
-        <v>17</v>
+      <c r="J479" s="1">
+        <v>0</v>
       </c>
       <c r="K479" s="1">
         <v>1</v>
@@ -21900,8 +21900,8 @@
       <c r="E480" s="1">
         <v>4</v>
       </c>
-      <c r="F480" s="1" t="s">
-        <v>17</v>
+      <c r="F480" s="1">
+        <v>0</v>
       </c>
       <c r="G480" s="1">
         <v>1</v>
@@ -21912,8 +21912,8 @@
       <c r="I480" s="1">
         <v>4</v>
       </c>
-      <c r="J480" s="1" t="s">
-        <v>17</v>
+      <c r="J480" s="1">
+        <v>0</v>
       </c>
       <c r="K480" s="1">
         <v>1</v>
@@ -21944,8 +21944,8 @@
       <c r="E481" s="1">
         <v>4</v>
       </c>
-      <c r="F481" s="1" t="s">
-        <v>17</v>
+      <c r="F481" s="1">
+        <v>0</v>
       </c>
       <c r="G481" s="1">
         <v>1</v>
@@ -21956,8 +21956,8 @@
       <c r="I481" s="1">
         <v>4</v>
       </c>
-      <c r="J481" s="1" t="s">
-        <v>17</v>
+      <c r="J481" s="1">
+        <v>0</v>
       </c>
       <c r="K481" s="1">
         <v>1</v>
@@ -21988,8 +21988,8 @@
       <c r="E482" s="1">
         <v>4</v>
       </c>
-      <c r="F482" s="1" t="s">
-        <v>17</v>
+      <c r="F482" s="1">
+        <v>0</v>
       </c>
       <c r="G482" s="1">
         <v>1</v>
@@ -22000,8 +22000,8 @@
       <c r="I482" s="1">
         <v>4</v>
       </c>
-      <c r="J482" s="1" t="s">
-        <v>17</v>
+      <c r="J482" s="1">
+        <v>0</v>
       </c>
       <c r="K482" s="1">
         <v>1</v>
@@ -22032,8 +22032,8 @@
       <c r="E483" s="1">
         <v>4</v>
       </c>
-      <c r="F483" s="1" t="s">
-        <v>17</v>
+      <c r="F483" s="1">
+        <v>0</v>
       </c>
       <c r="G483" s="1">
         <v>1</v>
@@ -22044,8 +22044,8 @@
       <c r="I483" s="1">
         <v>4</v>
       </c>
-      <c r="J483" s="1" t="s">
-        <v>17</v>
+      <c r="J483" s="1">
+        <v>0</v>
       </c>
       <c r="K483" s="1">
         <v>1</v>
@@ -22076,8 +22076,8 @@
       <c r="E484" s="1">
         <v>4</v>
       </c>
-      <c r="F484" s="1" t="s">
-        <v>17</v>
+      <c r="F484" s="1">
+        <v>0</v>
       </c>
       <c r="G484" s="1">
         <v>1</v>
@@ -22088,8 +22088,8 @@
       <c r="I484" s="1">
         <v>4</v>
       </c>
-      <c r="J484" s="1" t="s">
-        <v>17</v>
+      <c r="J484" s="1">
+        <v>0</v>
       </c>
       <c r="K484" s="1">
         <v>1</v>
@@ -22120,8 +22120,8 @@
       <c r="E485" s="1">
         <v>4</v>
       </c>
-      <c r="F485" s="1" t="s">
-        <v>17</v>
+      <c r="F485" s="1">
+        <v>0</v>
       </c>
       <c r="G485" s="1">
         <v>1</v>
@@ -22132,8 +22132,8 @@
       <c r="I485" s="1">
         <v>4</v>
       </c>
-      <c r="J485" s="1" t="s">
-        <v>17</v>
+      <c r="J485" s="1">
+        <v>0</v>
       </c>
       <c r="K485" s="1">
         <v>1</v>
@@ -22164,8 +22164,8 @@
       <c r="E486" s="1">
         <v>4</v>
       </c>
-      <c r="F486" s="1" t="s">
-        <v>17</v>
+      <c r="F486" s="1">
+        <v>0</v>
       </c>
       <c r="G486" s="1">
         <v>1</v>
@@ -22176,8 +22176,8 @@
       <c r="I486" s="1">
         <v>4</v>
       </c>
-      <c r="J486" s="1" t="s">
-        <v>17</v>
+      <c r="J486" s="1">
+        <v>0</v>
       </c>
       <c r="K486" s="1">
         <v>1</v>
@@ -22208,8 +22208,8 @@
       <c r="E487" s="1">
         <v>4</v>
       </c>
-      <c r="F487" s="1" t="s">
-        <v>17</v>
+      <c r="F487" s="1">
+        <v>0</v>
       </c>
       <c r="G487" s="1">
         <v>1</v>
@@ -22220,8 +22220,8 @@
       <c r="I487" s="1">
         <v>4</v>
       </c>
-      <c r="J487" s="1" t="s">
-        <v>17</v>
+      <c r="J487" s="1">
+        <v>0</v>
       </c>
       <c r="K487" s="1">
         <v>1</v>
@@ -22252,8 +22252,8 @@
       <c r="E488" s="1">
         <v>4</v>
       </c>
-      <c r="F488" s="1" t="s">
-        <v>17</v>
+      <c r="F488" s="1">
+        <v>0</v>
       </c>
       <c r="G488" s="1">
         <v>1</v>
@@ -22264,8 +22264,8 @@
       <c r="I488" s="1">
         <v>4</v>
       </c>
-      <c r="J488" s="1" t="s">
-        <v>17</v>
+      <c r="J488" s="1">
+        <v>0</v>
       </c>
       <c r="K488" s="1">
         <v>1</v>
@@ -22296,8 +22296,8 @@
       <c r="E489" s="1">
         <v>4</v>
       </c>
-      <c r="F489" s="1" t="s">
-        <v>17</v>
+      <c r="F489" s="1">
+        <v>0</v>
       </c>
       <c r="G489" s="1">
         <v>1</v>
@@ -22308,8 +22308,8 @@
       <c r="I489" s="1">
         <v>4</v>
       </c>
-      <c r="J489" s="1" t="s">
-        <v>17</v>
+      <c r="J489" s="1">
+        <v>0</v>
       </c>
       <c r="K489" s="1">
         <v>1</v>
@@ -22340,8 +22340,8 @@
       <c r="E490" s="1">
         <v>4</v>
       </c>
-      <c r="F490" s="1" t="s">
-        <v>17</v>
+      <c r="F490" s="1">
+        <v>0</v>
       </c>
       <c r="G490" s="1">
         <v>1</v>
@@ -22352,8 +22352,8 @@
       <c r="I490" s="1">
         <v>4</v>
       </c>
-      <c r="J490" s="1" t="s">
-        <v>17</v>
+      <c r="J490" s="1">
+        <v>0</v>
       </c>
       <c r="K490" s="1">
         <v>1</v>
@@ -22384,8 +22384,8 @@
       <c r="E491" s="1">
         <v>4</v>
       </c>
-      <c r="F491" s="1" t="s">
-        <v>17</v>
+      <c r="F491" s="1">
+        <v>0</v>
       </c>
       <c r="G491" s="1">
         <v>1</v>
@@ -22396,8 +22396,8 @@
       <c r="I491" s="1">
         <v>4</v>
       </c>
-      <c r="J491" s="1" t="s">
-        <v>17</v>
+      <c r="J491" s="1">
+        <v>0</v>
       </c>
       <c r="K491" s="1">
         <v>1</v>
@@ -22428,8 +22428,8 @@
       <c r="E492" s="1">
         <v>4</v>
       </c>
-      <c r="F492" s="1" t="s">
-        <v>17</v>
+      <c r="F492" s="1">
+        <v>0</v>
       </c>
       <c r="G492" s="1">
         <v>1</v>
@@ -22440,8 +22440,8 @@
       <c r="I492" s="1">
         <v>4</v>
       </c>
-      <c r="J492" s="1" t="s">
-        <v>17</v>
+      <c r="J492" s="1">
+        <v>0</v>
       </c>
       <c r="K492" s="1">
         <v>1</v>
@@ -22472,8 +22472,8 @@
       <c r="E493" s="1">
         <v>4</v>
       </c>
-      <c r="F493" s="1" t="s">
-        <v>17</v>
+      <c r="F493" s="1">
+        <v>0</v>
       </c>
       <c r="G493" s="1">
         <v>1</v>
@@ -22484,8 +22484,8 @@
       <c r="I493" s="1">
         <v>4</v>
       </c>
-      <c r="J493" s="1" t="s">
-        <v>17</v>
+      <c r="J493" s="1">
+        <v>0</v>
       </c>
       <c r="K493" s="1">
         <v>1</v>
@@ -22516,8 +22516,8 @@
       <c r="E494" s="1">
         <v>4</v>
       </c>
-      <c r="F494" s="1" t="s">
-        <v>17</v>
+      <c r="F494" s="1">
+        <v>0</v>
       </c>
       <c r="G494" s="1">
         <v>1</v>
@@ -22528,8 +22528,8 @@
       <c r="I494" s="1">
         <v>4</v>
       </c>
-      <c r="J494" s="1" t="s">
-        <v>17</v>
+      <c r="J494" s="1">
+        <v>0</v>
       </c>
       <c r="K494" s="1">
         <v>1</v>
@@ -22560,8 +22560,8 @@
       <c r="E495" s="1">
         <v>4</v>
       </c>
-      <c r="F495" s="1" t="s">
-        <v>17</v>
+      <c r="F495" s="1">
+        <v>0</v>
       </c>
       <c r="G495" s="1">
         <v>1</v>
@@ -22572,8 +22572,8 @@
       <c r="I495" s="1">
         <v>4</v>
       </c>
-      <c r="J495" s="1" t="s">
-        <v>17</v>
+      <c r="J495" s="1">
+        <v>0</v>
       </c>
       <c r="K495" s="1">
         <v>1</v>
@@ -22604,8 +22604,8 @@
       <c r="E496" s="1">
         <v>4</v>
       </c>
-      <c r="F496" s="1" t="s">
-        <v>17</v>
+      <c r="F496" s="1">
+        <v>0</v>
       </c>
       <c r="G496" s="1">
         <v>1</v>
@@ -22616,8 +22616,8 @@
       <c r="I496" s="1">
         <v>4</v>
       </c>
-      <c r="J496" s="1" t="s">
-        <v>17</v>
+      <c r="J496" s="1">
+        <v>0</v>
       </c>
       <c r="K496" s="1">
         <v>1</v>
@@ -22648,8 +22648,8 @@
       <c r="E497" s="1">
         <v>4</v>
       </c>
-      <c r="F497" s="1" t="s">
-        <v>17</v>
+      <c r="F497" s="1">
+        <v>0</v>
       </c>
       <c r="G497" s="1">
         <v>1</v>
@@ -22660,8 +22660,8 @@
       <c r="I497" s="1">
         <v>4</v>
       </c>
-      <c r="J497" s="1" t="s">
-        <v>17</v>
+      <c r="J497" s="1">
+        <v>0</v>
       </c>
       <c r="K497" s="1">
         <v>1</v>
@@ -22692,8 +22692,8 @@
       <c r="E498" s="1">
         <v>4</v>
       </c>
-      <c r="F498" s="1" t="s">
-        <v>17</v>
+      <c r="F498" s="1">
+        <v>0</v>
       </c>
       <c r="G498" s="1">
         <v>1</v>
@@ -22704,8 +22704,8 @@
       <c r="I498" s="1">
         <v>4</v>
       </c>
-      <c r="J498" s="1" t="s">
-        <v>17</v>
+      <c r="J498" s="1">
+        <v>0</v>
       </c>
       <c r="K498" s="1">
         <v>1</v>
@@ -22736,8 +22736,8 @@
       <c r="E499" s="1">
         <v>4</v>
       </c>
-      <c r="F499" s="1" t="s">
-        <v>17</v>
+      <c r="F499" s="1">
+        <v>0</v>
       </c>
       <c r="G499" s="1">
         <v>1</v>
@@ -22748,8 +22748,8 @@
       <c r="I499" s="1">
         <v>4</v>
       </c>
-      <c r="J499" s="1" t="s">
-        <v>17</v>
+      <c r="J499" s="1">
+        <v>0</v>
       </c>
       <c r="K499" s="1">
         <v>1</v>
@@ -22780,8 +22780,8 @@
       <c r="E500" s="1">
         <v>4</v>
       </c>
-      <c r="F500" s="1" t="s">
-        <v>17</v>
+      <c r="F500" s="1">
+        <v>0</v>
       </c>
       <c r="G500" s="1">
         <v>1</v>
@@ -22792,8 +22792,8 @@
       <c r="I500" s="1">
         <v>4</v>
       </c>
-      <c r="J500" s="1" t="s">
-        <v>17</v>
+      <c r="J500" s="1">
+        <v>0</v>
       </c>
       <c r="K500" s="1">
         <v>1</v>
@@ -22824,8 +22824,8 @@
       <c r="E501" s="1">
         <v>4</v>
       </c>
-      <c r="F501" s="1" t="s">
-        <v>17</v>
+      <c r="F501" s="1">
+        <v>0</v>
       </c>
       <c r="G501" s="1">
         <v>1</v>
@@ -22836,8 +22836,8 @@
       <c r="I501" s="1">
         <v>4</v>
       </c>
-      <c r="J501" s="1" t="s">
-        <v>17</v>
+      <c r="J501" s="1">
+        <v>0</v>
       </c>
       <c r="K501" s="1">
         <v>1</v>
@@ -22868,8 +22868,8 @@
       <c r="E502" s="1">
         <v>4</v>
       </c>
-      <c r="F502" s="1" t="s">
-        <v>17</v>
+      <c r="F502" s="1">
+        <v>0</v>
       </c>
       <c r="G502" s="1">
         <v>1</v>
@@ -22880,8 +22880,8 @@
       <c r="I502" s="1">
         <v>4</v>
       </c>
-      <c r="J502" s="1" t="s">
-        <v>17</v>
+      <c r="J502" s="1">
+        <v>0</v>
       </c>
       <c r="K502" s="1">
         <v>1</v>
@@ -22912,8 +22912,8 @@
       <c r="E503" s="1">
         <v>4</v>
       </c>
-      <c r="F503" s="1" t="s">
-        <v>17</v>
+      <c r="F503" s="1">
+        <v>0</v>
       </c>
       <c r="G503" s="1">
         <v>1</v>
@@ -22924,8 +22924,8 @@
       <c r="I503" s="1">
         <v>4</v>
       </c>
-      <c r="J503" s="1" t="s">
-        <v>17</v>
+      <c r="J503" s="1">
+        <v>0</v>
       </c>
       <c r="K503" s="1">
         <v>1</v>
@@ -22956,8 +22956,8 @@
       <c r="E504" s="1">
         <v>4</v>
       </c>
-      <c r="F504" s="1" t="s">
-        <v>17</v>
+      <c r="F504" s="1">
+        <v>0</v>
       </c>
       <c r="G504" s="1">
         <v>1</v>
@@ -22968,8 +22968,8 @@
       <c r="I504" s="1">
         <v>4</v>
       </c>
-      <c r="J504" s="1" t="s">
-        <v>17</v>
+      <c r="J504" s="1">
+        <v>0</v>
       </c>
       <c r="K504" s="1">
         <v>1</v>
@@ -23000,8 +23000,8 @@
       <c r="E505" s="1">
         <v>4</v>
       </c>
-      <c r="F505" s="1" t="s">
-        <v>17</v>
+      <c r="F505" s="1">
+        <v>0</v>
       </c>
       <c r="G505" s="1">
         <v>1</v>
@@ -23012,8 +23012,8 @@
       <c r="I505" s="1">
         <v>4</v>
       </c>
-      <c r="J505" s="1" t="s">
-        <v>17</v>
+      <c r="J505" s="1">
+        <v>0</v>
       </c>
       <c r="K505" s="1">
         <v>1</v>
@@ -23044,8 +23044,8 @@
       <c r="E506" s="1">
         <v>4</v>
       </c>
-      <c r="F506" s="1" t="s">
-        <v>17</v>
+      <c r="F506" s="1">
+        <v>0</v>
       </c>
       <c r="G506" s="1">
         <v>1</v>
@@ -23056,8 +23056,8 @@
       <c r="I506" s="1">
         <v>4</v>
       </c>
-      <c r="J506" s="1" t="s">
-        <v>17</v>
+      <c r="J506" s="1">
+        <v>0</v>
       </c>
       <c r="K506" s="1">
         <v>1</v>
@@ -23088,8 +23088,8 @@
       <c r="E507" s="1">
         <v>4</v>
       </c>
-      <c r="F507" s="1" t="s">
-        <v>17</v>
+      <c r="F507" s="1">
+        <v>0</v>
       </c>
       <c r="G507" s="1">
         <v>1</v>
@@ -23100,8 +23100,8 @@
       <c r="I507" s="1">
         <v>4</v>
       </c>
-      <c r="J507" s="1" t="s">
-        <v>17</v>
+      <c r="J507" s="1">
+        <v>0</v>
       </c>
       <c r="K507" s="1">
         <v>1</v>
@@ -23132,8 +23132,8 @@
       <c r="E508" s="1">
         <v>4</v>
       </c>
-      <c r="F508" s="1" t="s">
-        <v>17</v>
+      <c r="F508" s="1">
+        <v>0</v>
       </c>
       <c r="G508" s="1">
         <v>1</v>
@@ -23144,8 +23144,8 @@
       <c r="I508" s="1">
         <v>4</v>
       </c>
-      <c r="J508" s="1" t="s">
-        <v>17</v>
+      <c r="J508" s="1">
+        <v>0</v>
       </c>
       <c r="K508" s="1">
         <v>1</v>
@@ -23176,8 +23176,8 @@
       <c r="E509" s="1">
         <v>4</v>
       </c>
-      <c r="F509" s="1" t="s">
-        <v>17</v>
+      <c r="F509" s="1">
+        <v>0</v>
       </c>
       <c r="G509" s="1">
         <v>1</v>
@@ -23188,8 +23188,8 @@
       <c r="I509" s="1">
         <v>4</v>
       </c>
-      <c r="J509" s="1" t="s">
-        <v>17</v>
+      <c r="J509" s="1">
+        <v>0</v>
       </c>
       <c r="K509" s="1">
         <v>1</v>
@@ -23220,8 +23220,8 @@
       <c r="E510" s="1">
         <v>4</v>
       </c>
-      <c r="F510" s="1" t="s">
-        <v>17</v>
+      <c r="F510" s="1">
+        <v>0</v>
       </c>
       <c r="G510" s="1">
         <v>1</v>
@@ -23232,8 +23232,8 @@
       <c r="I510" s="1">
         <v>4</v>
       </c>
-      <c r="J510" s="1" t="s">
-        <v>17</v>
+      <c r="J510" s="1">
+        <v>0</v>
       </c>
       <c r="K510" s="1">
         <v>1</v>
@@ -23264,8 +23264,8 @@
       <c r="E511" s="1">
         <v>4</v>
       </c>
-      <c r="F511" s="1" t="s">
-        <v>17</v>
+      <c r="F511" s="1">
+        <v>0</v>
       </c>
       <c r="G511" s="1">
         <v>1</v>
@@ -23276,8 +23276,8 @@
       <c r="I511" s="1">
         <v>4</v>
       </c>
-      <c r="J511" s="1" t="s">
-        <v>17</v>
+      <c r="J511" s="1">
+        <v>0</v>
       </c>
       <c r="K511" s="1">
         <v>1</v>
@@ -23308,8 +23308,8 @@
       <c r="E512" s="1">
         <v>4</v>
       </c>
-      <c r="F512" s="1" t="s">
-        <v>17</v>
+      <c r="F512" s="1">
+        <v>0</v>
       </c>
       <c r="G512" s="1">
         <v>1</v>
@@ -23320,8 +23320,8 @@
       <c r="I512" s="1">
         <v>4</v>
       </c>
-      <c r="J512" s="1" t="s">
-        <v>17</v>
+      <c r="J512" s="1">
+        <v>0</v>
       </c>
       <c r="K512" s="1">
         <v>1</v>
@@ -23352,8 +23352,8 @@
       <c r="E513" s="1">
         <v>4</v>
       </c>
-      <c r="F513" s="1" t="s">
-        <v>17</v>
+      <c r="F513" s="1">
+        <v>0</v>
       </c>
       <c r="G513" s="1">
         <v>1</v>
@@ -23364,8 +23364,8 @@
       <c r="I513" s="1">
         <v>4</v>
       </c>
-      <c r="J513" s="1" t="s">
-        <v>17</v>
+      <c r="J513" s="1">
+        <v>0</v>
       </c>
       <c r="K513" s="1">
         <v>1</v>
@@ -23396,8 +23396,8 @@
       <c r="E514" s="1">
         <v>4</v>
       </c>
-      <c r="F514" s="1" t="s">
-        <v>17</v>
+      <c r="F514" s="1">
+        <v>0</v>
       </c>
       <c r="G514" s="1">
         <v>1</v>
@@ -23408,8 +23408,8 @@
       <c r="I514" s="1">
         <v>4</v>
       </c>
-      <c r="J514" s="1" t="s">
-        <v>17</v>
+      <c r="J514" s="1">
+        <v>0</v>
       </c>
       <c r="K514" s="1">
         <v>1</v>
@@ -23440,8 +23440,8 @@
       <c r="E515" s="1">
         <v>4</v>
       </c>
-      <c r="F515" s="1" t="s">
-        <v>17</v>
+      <c r="F515" s="1">
+        <v>0</v>
       </c>
       <c r="G515" s="1">
         <v>1</v>
@@ -23452,8 +23452,8 @@
       <c r="I515" s="1">
         <v>4</v>
       </c>
-      <c r="J515" s="1" t="s">
-        <v>17</v>
+      <c r="J515" s="1">
+        <v>0</v>
       </c>
       <c r="K515" s="1">
         <v>1</v>
@@ -23484,8 +23484,8 @@
       <c r="E516" s="1">
         <v>4</v>
       </c>
-      <c r="F516" s="1" t="s">
-        <v>17</v>
+      <c r="F516" s="1">
+        <v>0</v>
       </c>
       <c r="G516" s="1">
         <v>1</v>
@@ -23496,8 +23496,8 @@
       <c r="I516" s="1">
         <v>4</v>
       </c>
-      <c r="J516" s="1" t="s">
-        <v>17</v>
+      <c r="J516" s="1">
+        <v>0</v>
       </c>
       <c r="K516" s="1">
         <v>1</v>
@@ -23528,8 +23528,8 @@
       <c r="E517" s="1">
         <v>4</v>
       </c>
-      <c r="F517" s="1" t="s">
-        <v>17</v>
+      <c r="F517" s="1">
+        <v>0</v>
       </c>
       <c r="G517" s="1">
         <v>1</v>
@@ -23540,8 +23540,8 @@
       <c r="I517" s="1">
         <v>4</v>
       </c>
-      <c r="J517" s="1" t="s">
-        <v>17</v>
+      <c r="J517" s="1">
+        <v>0</v>
       </c>
       <c r="K517" s="1">
         <v>1</v>
@@ -23572,8 +23572,8 @@
       <c r="E518" s="1">
         <v>4</v>
       </c>
-      <c r="F518" s="1" t="s">
-        <v>17</v>
+      <c r="F518" s="1">
+        <v>0</v>
       </c>
       <c r="G518" s="1">
         <v>1</v>
@@ -23584,8 +23584,8 @@
       <c r="I518" s="1">
         <v>4</v>
       </c>
-      <c r="J518" s="1" t="s">
-        <v>17</v>
+      <c r="J518" s="1">
+        <v>0</v>
       </c>
       <c r="K518" s="1">
         <v>1</v>
@@ -23616,8 +23616,8 @@
       <c r="E519" s="1">
         <v>4</v>
       </c>
-      <c r="F519" s="1" t="s">
-        <v>17</v>
+      <c r="F519" s="1">
+        <v>0</v>
       </c>
       <c r="G519" s="1">
         <v>1</v>
@@ -23628,8 +23628,8 @@
       <c r="I519" s="1">
         <v>4</v>
       </c>
-      <c r="J519" s="1" t="s">
-        <v>17</v>
+      <c r="J519" s="1">
+        <v>0</v>
       </c>
       <c r="K519" s="1">
         <v>1</v>
@@ -23660,8 +23660,8 @@
       <c r="E520" s="1">
         <v>4</v>
       </c>
-      <c r="F520" s="1" t="s">
-        <v>17</v>
+      <c r="F520" s="1">
+        <v>0</v>
       </c>
       <c r="G520" s="1">
         <v>1</v>
@@ -23672,8 +23672,8 @@
       <c r="I520" s="1">
         <v>4</v>
       </c>
-      <c r="J520" s="1" t="s">
-        <v>17</v>
+      <c r="J520" s="1">
+        <v>0</v>
       </c>
       <c r="K520" s="1">
         <v>1</v>
@@ -23704,8 +23704,8 @@
       <c r="E521" s="1">
         <v>4</v>
       </c>
-      <c r="F521" s="1" t="s">
-        <v>17</v>
+      <c r="F521" s="1">
+        <v>0</v>
       </c>
       <c r="G521" s="1">
         <v>1</v>
@@ -23716,8 +23716,8 @@
       <c r="I521" s="1">
         <v>4</v>
       </c>
-      <c r="J521" s="1" t="s">
-        <v>17</v>
+      <c r="J521" s="1">
+        <v>0</v>
       </c>
       <c r="K521" s="1">
         <v>1</v>
@@ -23748,8 +23748,8 @@
       <c r="E522" s="1">
         <v>4</v>
       </c>
-      <c r="F522" s="1" t="s">
-        <v>17</v>
+      <c r="F522" s="1">
+        <v>0</v>
       </c>
       <c r="G522" s="1">
         <v>1</v>
@@ -23760,8 +23760,8 @@
       <c r="I522" s="1">
         <v>4</v>
       </c>
-      <c r="J522" s="1" t="s">
-        <v>17</v>
+      <c r="J522" s="1">
+        <v>0</v>
       </c>
       <c r="K522" s="1">
         <v>1</v>
@@ -23792,8 +23792,8 @@
       <c r="E523" s="1">
         <v>4</v>
       </c>
-      <c r="F523" s="1" t="s">
-        <v>17</v>
+      <c r="F523" s="1">
+        <v>0</v>
       </c>
       <c r="G523" s="1">
         <v>1</v>
@@ -23804,8 +23804,8 @@
       <c r="I523" s="1">
         <v>4</v>
       </c>
-      <c r="J523" s="1" t="s">
-        <v>17</v>
+      <c r="J523" s="1">
+        <v>0</v>
       </c>
       <c r="K523" s="1">
         <v>1</v>
@@ -23836,8 +23836,8 @@
       <c r="E524" s="1">
         <v>4</v>
       </c>
-      <c r="F524" s="1" t="s">
-        <v>17</v>
+      <c r="F524" s="1">
+        <v>0</v>
       </c>
       <c r="G524" s="1">
         <v>1</v>
@@ -23848,8 +23848,8 @@
       <c r="I524" s="1">
         <v>4</v>
       </c>
-      <c r="J524" s="1" t="s">
-        <v>17</v>
+      <c r="J524" s="1">
+        <v>0</v>
       </c>
       <c r="K524" s="1">
         <v>1</v>
@@ -23880,8 +23880,8 @@
       <c r="E525" s="1">
         <v>4</v>
       </c>
-      <c r="F525" s="1" t="s">
-        <v>17</v>
+      <c r="F525" s="1">
+        <v>0</v>
       </c>
       <c r="G525" s="1">
         <v>1</v>
@@ -23892,8 +23892,8 @@
       <c r="I525" s="1">
         <v>4</v>
       </c>
-      <c r="J525" s="1" t="s">
-        <v>17</v>
+      <c r="J525" s="1">
+        <v>0</v>
       </c>
       <c r="K525" s="1">
         <v>1</v>
@@ -23924,8 +23924,8 @@
       <c r="E526" s="1">
         <v>4</v>
       </c>
-      <c r="F526" s="1" t="s">
-        <v>17</v>
+      <c r="F526" s="1">
+        <v>0</v>
       </c>
       <c r="G526" s="1">
         <v>1</v>
@@ -23936,8 +23936,8 @@
       <c r="I526" s="1">
         <v>4</v>
       </c>
-      <c r="J526" s="1" t="s">
-        <v>17</v>
+      <c r="J526" s="1">
+        <v>0</v>
       </c>
       <c r="K526" s="1">
         <v>1</v>
@@ -23968,8 +23968,8 @@
       <c r="E527" s="1">
         <v>4</v>
       </c>
-      <c r="F527" s="1" t="s">
-        <v>17</v>
+      <c r="F527" s="1">
+        <v>0</v>
       </c>
       <c r="G527" s="1">
         <v>1</v>
@@ -23980,8 +23980,8 @@
       <c r="I527" s="1">
         <v>4</v>
       </c>
-      <c r="J527" s="1" t="s">
-        <v>17</v>
+      <c r="J527" s="1">
+        <v>0</v>
       </c>
       <c r="K527" s="1">
         <v>1</v>
@@ -24012,8 +24012,8 @@
       <c r="E528" s="1">
         <v>4</v>
       </c>
-      <c r="F528" s="1" t="s">
-        <v>17</v>
+      <c r="F528" s="1">
+        <v>0</v>
       </c>
       <c r="G528" s="1">
         <v>1</v>
@@ -24024,8 +24024,8 @@
       <c r="I528" s="1">
         <v>4</v>
       </c>
-      <c r="J528" s="1" t="s">
-        <v>17</v>
+      <c r="J528" s="1">
+        <v>0</v>
       </c>
       <c r="K528" s="1">
         <v>1</v>
@@ -24056,8 +24056,8 @@
       <c r="E529" s="1">
         <v>4</v>
       </c>
-      <c r="F529" s="1" t="s">
-        <v>17</v>
+      <c r="F529" s="1">
+        <v>0</v>
       </c>
       <c r="G529" s="1">
         <v>1</v>
@@ -24068,8 +24068,8 @@
       <c r="I529" s="1">
         <v>4</v>
       </c>
-      <c r="J529" s="1" t="s">
-        <v>17</v>
+      <c r="J529" s="1">
+        <v>0</v>
       </c>
       <c r="K529" s="1">
         <v>1</v>
@@ -24100,8 +24100,8 @@
       <c r="E530" s="1">
         <v>4</v>
       </c>
-      <c r="F530" s="1" t="s">
-        <v>17</v>
+      <c r="F530" s="1">
+        <v>0</v>
       </c>
       <c r="G530" s="1">
         <v>1</v>
@@ -24112,8 +24112,8 @@
       <c r="I530" s="1">
         <v>4</v>
       </c>
-      <c r="J530" s="1" t="s">
-        <v>17</v>
+      <c r="J530" s="1">
+        <v>0</v>
       </c>
       <c r="K530" s="1">
         <v>1</v>
@@ -24144,8 +24144,8 @@
       <c r="E531" s="1">
         <v>4</v>
       </c>
-      <c r="F531" s="1" t="s">
-        <v>17</v>
+      <c r="F531" s="1">
+        <v>0</v>
       </c>
       <c r="G531" s="1">
         <v>1</v>
@@ -24156,8 +24156,8 @@
       <c r="I531" s="1">
         <v>4</v>
       </c>
-      <c r="J531" s="1" t="s">
-        <v>17</v>
+      <c r="J531" s="1">
+        <v>0</v>
       </c>
       <c r="K531" s="1">
         <v>1</v>
@@ -24188,8 +24188,8 @@
       <c r="E532" s="1">
         <v>4</v>
       </c>
-      <c r="F532" s="1" t="s">
-        <v>17</v>
+      <c r="F532" s="1">
+        <v>0</v>
       </c>
       <c r="G532" s="1">
         <v>1</v>
@@ -24200,8 +24200,8 @@
       <c r="I532" s="1">
         <v>4</v>
       </c>
-      <c r="J532" s="1" t="s">
-        <v>17</v>
+      <c r="J532" s="1">
+        <v>0</v>
       </c>
       <c r="K532" s="1">
         <v>1</v>
@@ -24232,8 +24232,8 @@
       <c r="E533" s="1">
         <v>4</v>
       </c>
-      <c r="F533" s="1" t="s">
-        <v>17</v>
+      <c r="F533" s="1">
+        <v>0</v>
       </c>
       <c r="G533" s="1">
         <v>1</v>
@@ -24244,8 +24244,8 @@
       <c r="I533" s="1">
         <v>4</v>
       </c>
-      <c r="J533" s="1" t="s">
-        <v>17</v>
+      <c r="J533" s="1">
+        <v>0</v>
       </c>
       <c r="K533" s="1">
         <v>1</v>
@@ -24276,8 +24276,8 @@
       <c r="E534" s="1">
         <v>4</v>
       </c>
-      <c r="F534" s="1" t="s">
-        <v>17</v>
+      <c r="F534" s="1">
+        <v>0</v>
       </c>
       <c r="G534" s="1">
         <v>1</v>
@@ -24288,8 +24288,8 @@
       <c r="I534" s="1">
         <v>4</v>
       </c>
-      <c r="J534" s="1" t="s">
-        <v>17</v>
+      <c r="J534" s="1">
+        <v>0</v>
       </c>
       <c r="K534" s="1">
         <v>1</v>
@@ -24320,8 +24320,8 @@
       <c r="E535" s="1">
         <v>4</v>
       </c>
-      <c r="F535" s="1" t="s">
-        <v>17</v>
+      <c r="F535" s="1">
+        <v>0</v>
       </c>
       <c r="G535" s="1">
         <v>1</v>
@@ -24332,8 +24332,8 @@
       <c r="I535" s="1">
         <v>4</v>
       </c>
-      <c r="J535" s="1" t="s">
-        <v>17</v>
+      <c r="J535" s="1">
+        <v>0</v>
       </c>
       <c r="K535" s="1">
         <v>1</v>
@@ -24364,8 +24364,8 @@
       <c r="E536" s="1">
         <v>4</v>
       </c>
-      <c r="F536" s="1" t="s">
-        <v>17</v>
+      <c r="F536" s="1">
+        <v>0</v>
       </c>
       <c r="G536" s="1">
         <v>1</v>
@@ -24376,8 +24376,8 @@
       <c r="I536" s="1">
         <v>4</v>
       </c>
-      <c r="J536" s="1" t="s">
-        <v>17</v>
+      <c r="J536" s="1">
+        <v>0</v>
       </c>
       <c r="K536" s="1">
         <v>1</v>
@@ -24408,8 +24408,8 @@
       <c r="E537" s="1">
         <v>4</v>
       </c>
-      <c r="F537" s="1" t="s">
-        <v>17</v>
+      <c r="F537" s="1">
+        <v>0</v>
       </c>
       <c r="G537" s="1">
         <v>1</v>
@@ -24420,8 +24420,8 @@
       <c r="I537" s="1">
         <v>4</v>
       </c>
-      <c r="J537" s="1" t="s">
-        <v>17</v>
+      <c r="J537" s="1">
+        <v>0</v>
       </c>
       <c r="K537" s="1">
         <v>1</v>
@@ -24452,8 +24452,8 @@
       <c r="E538" s="1">
         <v>4</v>
       </c>
-      <c r="F538" s="1" t="s">
-        <v>17</v>
+      <c r="F538" s="1">
+        <v>0</v>
       </c>
       <c r="G538" s="1">
         <v>1</v>
@@ -24464,8 +24464,8 @@
       <c r="I538" s="1">
         <v>4</v>
       </c>
-      <c r="J538" s="1" t="s">
-        <v>17</v>
+      <c r="J538" s="1">
+        <v>0</v>
       </c>
       <c r="K538" s="1">
         <v>1</v>
@@ -24496,8 +24496,8 @@
       <c r="E539" s="1">
         <v>4</v>
       </c>
-      <c r="F539" s="1" t="s">
-        <v>17</v>
+      <c r="F539" s="1">
+        <v>0</v>
       </c>
       <c r="G539" s="1">
         <v>1</v>
@@ -24508,8 +24508,8 @@
       <c r="I539" s="1">
         <v>4</v>
       </c>
-      <c r="J539" s="1" t="s">
-        <v>17</v>
+      <c r="J539" s="1">
+        <v>0</v>
       </c>
       <c r="K539" s="1">
         <v>1</v>
@@ -24540,8 +24540,8 @@
       <c r="E540" s="1">
         <v>4</v>
       </c>
-      <c r="F540" s="1" t="s">
-        <v>17</v>
+      <c r="F540" s="1">
+        <v>0</v>
       </c>
       <c r="G540" s="1">
         <v>1</v>
@@ -24552,8 +24552,8 @@
       <c r="I540" s="1">
         <v>4</v>
       </c>
-      <c r="J540" s="1" t="s">
-        <v>17</v>
+      <c r="J540" s="1">
+        <v>0</v>
       </c>
       <c r="K540" s="1">
         <v>1</v>
@@ -24584,8 +24584,8 @@
       <c r="E541" s="1">
         <v>4</v>
       </c>
-      <c r="F541" s="1" t="s">
-        <v>17</v>
+      <c r="F541" s="1">
+        <v>0</v>
       </c>
       <c r="G541" s="1">
         <v>1</v>
@@ -24596,8 +24596,8 @@
       <c r="I541" s="1">
         <v>4</v>
       </c>
-      <c r="J541" s="1" t="s">
-        <v>17</v>
+      <c r="J541" s="1">
+        <v>0</v>
       </c>
       <c r="K541" s="1">
         <v>1</v>
@@ -24628,8 +24628,8 @@
       <c r="E542" s="1">
         <v>4</v>
       </c>
-      <c r="F542" s="1" t="s">
-        <v>17</v>
+      <c r="F542" s="1">
+        <v>0</v>
       </c>
       <c r="G542" s="1">
         <v>1</v>
@@ -24640,8 +24640,8 @@
       <c r="I542" s="1">
         <v>4</v>
       </c>
-      <c r="J542" s="1" t="s">
-        <v>17</v>
+      <c r="J542" s="1">
+        <v>0</v>
       </c>
       <c r="K542" s="1">
         <v>1</v>
@@ -24672,8 +24672,8 @@
       <c r="E543" s="1">
         <v>4</v>
       </c>
-      <c r="F543" s="1" t="s">
-        <v>17</v>
+      <c r="F543" s="1">
+        <v>0</v>
       </c>
       <c r="G543" s="1">
         <v>1</v>
@@ -24684,8 +24684,8 @@
       <c r="I543" s="1">
         <v>4</v>
       </c>
-      <c r="J543" s="1" t="s">
-        <v>17</v>
+      <c r="J543" s="1">
+        <v>0</v>
       </c>
       <c r="K543" s="1">
         <v>1</v>
@@ -24716,8 +24716,8 @@
       <c r="E544" s="1">
         <v>4</v>
       </c>
-      <c r="F544" s="1" t="s">
-        <v>17</v>
+      <c r="F544" s="1">
+        <v>0</v>
       </c>
       <c r="G544" s="1">
         <v>1</v>
@@ -24728,8 +24728,8 @@
       <c r="I544" s="1">
         <v>4</v>
       </c>
-      <c r="J544" s="1" t="s">
-        <v>17</v>
+      <c r="J544" s="1">
+        <v>0</v>
       </c>
       <c r="K544" s="1">
         <v>1</v>
@@ -24760,8 +24760,8 @@
       <c r="E545" s="1">
         <v>4</v>
       </c>
-      <c r="F545" s="1" t="s">
-        <v>17</v>
+      <c r="F545" s="1">
+        <v>0</v>
       </c>
       <c r="G545" s="1">
         <v>1</v>
@@ -24772,8 +24772,8 @@
       <c r="I545" s="1">
         <v>4</v>
       </c>
-      <c r="J545" s="1" t="s">
-        <v>17</v>
+      <c r="J545" s="1">
+        <v>0</v>
       </c>
       <c r="K545" s="1">
         <v>1</v>
@@ -24804,8 +24804,8 @@
       <c r="E546" s="1">
         <v>4</v>
       </c>
-      <c r="F546" s="1" t="s">
-        <v>17</v>
+      <c r="F546" s="1">
+        <v>0</v>
       </c>
       <c r="G546" s="1">
         <v>1</v>
@@ -24816,8 +24816,8 @@
       <c r="I546" s="1">
         <v>4</v>
       </c>
-      <c r="J546" s="1" t="s">
-        <v>17</v>
+      <c r="J546" s="1">
+        <v>0</v>
       </c>
       <c r="K546" s="1">
         <v>1</v>
@@ -24848,8 +24848,8 @@
       <c r="E547" s="1">
         <v>4</v>
       </c>
-      <c r="F547" s="1" t="s">
-        <v>17</v>
+      <c r="F547" s="1">
+        <v>0</v>
       </c>
       <c r="G547" s="1">
         <v>1</v>
@@ -24860,8 +24860,8 @@
       <c r="I547" s="1">
         <v>4</v>
       </c>
-      <c r="J547" s="1" t="s">
-        <v>17</v>
+      <c r="J547" s="1">
+        <v>0</v>
       </c>
       <c r="K547" s="1">
         <v>1</v>
@@ -24892,8 +24892,8 @@
       <c r="E548" s="1">
         <v>4</v>
       </c>
-      <c r="F548" s="1" t="s">
-        <v>17</v>
+      <c r="F548" s="1">
+        <v>0</v>
       </c>
       <c r="G548" s="1">
         <v>1</v>
@@ -24904,8 +24904,8 @@
       <c r="I548" s="1">
         <v>4</v>
       </c>
-      <c r="J548" s="1" t="s">
-        <v>17</v>
+      <c r="J548" s="1">
+        <v>0</v>
       </c>
       <c r="K548" s="1">
         <v>1</v>
@@ -24936,8 +24936,8 @@
       <c r="E549" s="1">
         <v>4</v>
       </c>
-      <c r="F549" s="1" t="s">
-        <v>17</v>
+      <c r="F549" s="1">
+        <v>0</v>
       </c>
       <c r="G549" s="1">
         <v>1</v>
@@ -24948,8 +24948,8 @@
       <c r="I549" s="1">
         <v>4</v>
       </c>
-      <c r="J549" s="1" t="s">
-        <v>17</v>
+      <c r="J549" s="1">
+        <v>0</v>
       </c>
       <c r="K549" s="1">
         <v>1</v>
@@ -24980,8 +24980,8 @@
       <c r="E550" s="1">
         <v>4</v>
       </c>
-      <c r="F550" s="1" t="s">
-        <v>17</v>
+      <c r="F550" s="1">
+        <v>0</v>
       </c>
       <c r="G550" s="1">
         <v>1</v>
@@ -24992,8 +24992,8 @@
       <c r="I550" s="1">
         <v>4</v>
       </c>
-      <c r="J550" s="1" t="s">
-        <v>17</v>
+      <c r="J550" s="1">
+        <v>0</v>
       </c>
       <c r="K550" s="1">
         <v>1</v>
@@ -25024,8 +25024,8 @@
       <c r="E551" s="1">
         <v>4</v>
       </c>
-      <c r="F551" s="1" t="s">
-        <v>17</v>
+      <c r="F551" s="1">
+        <v>0</v>
       </c>
       <c r="G551" s="1">
         <v>1</v>
@@ -25036,8 +25036,8 @@
       <c r="I551" s="1">
         <v>4</v>
       </c>
-      <c r="J551" s="1" t="s">
-        <v>17</v>
+      <c r="J551" s="1">
+        <v>0</v>
       </c>
       <c r="K551" s="1">
         <v>1</v>
@@ -25068,8 +25068,8 @@
       <c r="E552" s="1">
         <v>4</v>
       </c>
-      <c r="F552" s="1" t="s">
-        <v>17</v>
+      <c r="F552" s="1">
+        <v>0</v>
       </c>
       <c r="G552" s="1">
         <v>1</v>
@@ -25080,8 +25080,8 @@
       <c r="I552" s="1">
         <v>4</v>
       </c>
-      <c r="J552" s="1" t="s">
-        <v>17</v>
+      <c r="J552" s="1">
+        <v>0</v>
       </c>
       <c r="K552" s="1">
         <v>1</v>
@@ -25112,8 +25112,8 @@
       <c r="E553" s="1">
         <v>4</v>
       </c>
-      <c r="F553" s="1" t="s">
-        <v>17</v>
+      <c r="F553" s="1">
+        <v>0</v>
       </c>
       <c r="G553" s="1">
         <v>1</v>
@@ -25124,8 +25124,8 @@
       <c r="I553" s="1">
         <v>4</v>
       </c>
-      <c r="J553" s="1" t="s">
-        <v>17</v>
+      <c r="J553" s="1">
+        <v>0</v>
       </c>
       <c r="K553" s="1">
         <v>1</v>
@@ -25156,8 +25156,8 @@
       <c r="E554" s="1">
         <v>4</v>
       </c>
-      <c r="F554" s="1" t="s">
-        <v>17</v>
+      <c r="F554" s="1">
+        <v>0</v>
       </c>
       <c r="G554" s="1">
         <v>1</v>
@@ -25168,8 +25168,8 @@
       <c r="I554" s="1">
         <v>4</v>
       </c>
-      <c r="J554" s="1" t="s">
-        <v>17</v>
+      <c r="J554" s="1">
+        <v>0</v>
       </c>
       <c r="K554" s="1">
         <v>1</v>
@@ -25200,8 +25200,8 @@
       <c r="E555" s="1">
         <v>4</v>
       </c>
-      <c r="F555" s="1" t="s">
-        <v>17</v>
+      <c r="F555" s="1">
+        <v>0</v>
       </c>
       <c r="G555" s="1">
         <v>1</v>
@@ -25212,8 +25212,8 @@
       <c r="I555" s="1">
         <v>4</v>
       </c>
-      <c r="J555" s="1" t="s">
-        <v>17</v>
+      <c r="J555" s="1">
+        <v>0</v>
       </c>
       <c r="K555" s="1">
         <v>1</v>
@@ -25244,8 +25244,8 @@
       <c r="E556" s="1">
         <v>4</v>
       </c>
-      <c r="F556" s="1" t="s">
-        <v>17</v>
+      <c r="F556" s="1">
+        <v>0</v>
       </c>
       <c r="G556" s="1">
         <v>1</v>
@@ -25256,8 +25256,8 @@
       <c r="I556" s="1">
         <v>4</v>
       </c>
-      <c r="J556" s="1" t="s">
-        <v>17</v>
+      <c r="J556" s="1">
+        <v>0</v>
       </c>
       <c r="K556" s="1">
         <v>1</v>
@@ -25288,8 +25288,8 @@
       <c r="E557" s="1">
         <v>4</v>
       </c>
-      <c r="F557" s="1" t="s">
-        <v>17</v>
+      <c r="F557" s="1">
+        <v>0</v>
       </c>
       <c r="G557" s="1">
         <v>1</v>
@@ -25300,8 +25300,8 @@
       <c r="I557" s="1">
         <v>4</v>
       </c>
-      <c r="J557" s="1" t="s">
-        <v>17</v>
+      <c r="J557" s="1">
+        <v>0</v>
       </c>
       <c r="K557" s="1">
         <v>1</v>
@@ -25332,8 +25332,8 @@
       <c r="E558" s="1">
         <v>4</v>
       </c>
-      <c r="F558" s="1" t="s">
-        <v>17</v>
+      <c r="F558" s="1">
+        <v>0</v>
       </c>
       <c r="G558" s="1">
         <v>1</v>
@@ -25344,8 +25344,8 @@
       <c r="I558" s="1">
         <v>4</v>
       </c>
-      <c r="J558" s="1" t="s">
-        <v>17</v>
+      <c r="J558" s="1">
+        <v>0</v>
       </c>
       <c r="K558" s="1">
         <v>1</v>
@@ -25376,8 +25376,8 @@
       <c r="E559" s="1">
         <v>4</v>
       </c>
-      <c r="F559" s="1" t="s">
-        <v>17</v>
+      <c r="F559" s="1">
+        <v>0</v>
       </c>
       <c r="G559" s="1">
         <v>1</v>
@@ -25388,8 +25388,8 @@
       <c r="I559" s="1">
         <v>4</v>
       </c>
-      <c r="J559" s="1" t="s">
-        <v>17</v>
+      <c r="J559" s="1">
+        <v>0</v>
       </c>
       <c r="K559" s="1">
         <v>1</v>
@@ -25420,8 +25420,8 @@
       <c r="E560" s="1">
         <v>4</v>
       </c>
-      <c r="F560" s="1" t="s">
-        <v>17</v>
+      <c r="F560" s="1">
+        <v>0</v>
       </c>
       <c r="G560" s="1">
         <v>1</v>
@@ -25432,8 +25432,8 @@
       <c r="I560" s="1">
         <v>4</v>
       </c>
-      <c r="J560" s="1" t="s">
-        <v>17</v>
+      <c r="J560" s="1">
+        <v>0</v>
       </c>
       <c r="K560" s="1">
         <v>1</v>
@@ -25464,8 +25464,8 @@
       <c r="E561" s="1">
         <v>4</v>
       </c>
-      <c r="F561" s="1" t="s">
-        <v>17</v>
+      <c r="F561" s="1">
+        <v>0</v>
       </c>
       <c r="G561" s="1">
         <v>1</v>
@@ -25476,8 +25476,8 @@
       <c r="I561" s="1">
         <v>4</v>
       </c>
-      <c r="J561" s="1" t="s">
-        <v>17</v>
+      <c r="J561" s="1">
+        <v>0</v>
       </c>
       <c r="K561" s="1">
         <v>1</v>
@@ -25508,8 +25508,8 @@
       <c r="E562" s="1">
         <v>4</v>
       </c>
-      <c r="F562" s="1" t="s">
-        <v>17</v>
+      <c r="F562" s="1">
+        <v>0</v>
       </c>
       <c r="G562" s="1">
         <v>1</v>
@@ -25520,8 +25520,8 @@
       <c r="I562" s="1">
         <v>4</v>
       </c>
-      <c r="J562" s="1" t="s">
-        <v>17</v>
+      <c r="J562" s="1">
+        <v>0</v>
       </c>
       <c r="K562" s="1">
         <v>1</v>
@@ -25552,8 +25552,8 @@
       <c r="E563" s="1">
         <v>4</v>
       </c>
-      <c r="F563" s="1" t="s">
-        <v>17</v>
+      <c r="F563" s="1">
+        <v>0</v>
       </c>
       <c r="G563" s="1">
         <v>1</v>
@@ -25564,8 +25564,8 @@
       <c r="I563" s="1">
         <v>4</v>
       </c>
-      <c r="J563" s="1" t="s">
-        <v>17</v>
+      <c r="J563" s="1">
+        <v>0</v>
       </c>
       <c r="K563" s="1">
         <v>1</v>
@@ -25596,8 +25596,8 @@
       <c r="E564" s="1">
         <v>4</v>
       </c>
-      <c r="F564" s="1" t="s">
-        <v>17</v>
+      <c r="F564" s="1">
+        <v>0</v>
       </c>
       <c r="G564" s="1">
         <v>1</v>
@@ -25608,8 +25608,8 @@
       <c r="I564" s="1">
         <v>4</v>
       </c>
-      <c r="J564" s="1" t="s">
-        <v>17</v>
+      <c r="J564" s="1">
+        <v>0</v>
       </c>
       <c r="K564" s="1">
         <v>1</v>
@@ -25640,8 +25640,8 @@
       <c r="E565" s="1">
         <v>4</v>
       </c>
-      <c r="F565" s="1" t="s">
-        <v>17</v>
+      <c r="F565" s="1">
+        <v>0</v>
       </c>
       <c r="G565" s="1">
         <v>1</v>
@@ -25652,8 +25652,8 @@
       <c r="I565" s="1">
         <v>4</v>
       </c>
-      <c r="J565" s="1" t="s">
-        <v>17</v>
+      <c r="J565" s="1">
+        <v>0</v>
       </c>
       <c r="K565" s="1">
         <v>1</v>
@@ -25684,8 +25684,8 @@
       <c r="E566" s="1">
         <v>4</v>
       </c>
-      <c r="F566" s="1" t="s">
-        <v>17</v>
+      <c r="F566" s="1">
+        <v>0</v>
       </c>
       <c r="G566" s="1">
         <v>1</v>
@@ -25696,8 +25696,8 @@
       <c r="I566" s="1">
         <v>4</v>
       </c>
-      <c r="J566" s="1" t="s">
-        <v>17</v>
+      <c r="J566" s="1">
+        <v>0</v>
       </c>
       <c r="K566" s="1">
         <v>1</v>
@@ -25728,8 +25728,8 @@
       <c r="E567" s="1">
         <v>4</v>
       </c>
-      <c r="F567" s="1" t="s">
-        <v>17</v>
+      <c r="F567" s="1">
+        <v>0</v>
       </c>
       <c r="G567" s="1">
         <v>1</v>
@@ -25740,8 +25740,8 @@
       <c r="I567" s="1">
         <v>4</v>
       </c>
-      <c r="J567" s="1" t="s">
-        <v>17</v>
+      <c r="J567" s="1">
+        <v>0</v>
       </c>
       <c r="K567" s="1">
         <v>1</v>
@@ -25772,8 +25772,8 @@
       <c r="E568" s="1">
         <v>4</v>
       </c>
-      <c r="F568" s="1" t="s">
-        <v>17</v>
+      <c r="F568" s="1">
+        <v>0</v>
       </c>
       <c r="G568" s="1">
         <v>1</v>
@@ -25784,8 +25784,8 @@
       <c r="I568" s="1">
         <v>4</v>
       </c>
-      <c r="J568" s="1" t="s">
-        <v>17</v>
+      <c r="J568" s="1">
+        <v>0</v>
       </c>
       <c r="K568" s="1">
         <v>1</v>
@@ -25816,8 +25816,8 @@
       <c r="E569" s="1">
         <v>4</v>
       </c>
-      <c r="F569" s="1" t="s">
-        <v>17</v>
+      <c r="F569" s="1">
+        <v>0</v>
       </c>
       <c r="G569" s="1">
         <v>1</v>
@@ -25828,8 +25828,8 @@
       <c r="I569" s="1">
         <v>4</v>
       </c>
-      <c r="J569" s="1" t="s">
-        <v>17</v>
+      <c r="J569" s="1">
+        <v>0</v>
       </c>
       <c r="K569" s="1">
         <v>1</v>
@@ -25860,8 +25860,8 @@
       <c r="E570" s="1">
         <v>4</v>
       </c>
-      <c r="F570" s="1" t="s">
-        <v>17</v>
+      <c r="F570" s="1">
+        <v>0</v>
       </c>
       <c r="G570" s="1">
         <v>1</v>
@@ -25872,8 +25872,8 @@
       <c r="I570" s="1">
         <v>4</v>
       </c>
-      <c r="J570" s="1" t="s">
-        <v>17</v>
+      <c r="J570" s="1">
+        <v>0</v>
       </c>
       <c r="K570" s="1">
         <v>1</v>
@@ -25904,8 +25904,8 @@
       <c r="E571" s="1">
         <v>4</v>
       </c>
-      <c r="F571" s="1" t="s">
-        <v>17</v>
+      <c r="F571" s="1">
+        <v>0</v>
       </c>
       <c r="G571" s="1">
         <v>1</v>
@@ -25916,8 +25916,8 @@
       <c r="I571" s="1">
         <v>4</v>
       </c>
-      <c r="J571" s="1" t="s">
-        <v>17</v>
+      <c r="J571" s="1">
+        <v>0</v>
       </c>
       <c r="K571" s="1">
         <v>1</v>
@@ -25948,8 +25948,8 @@
       <c r="E572" s="1">
         <v>4</v>
       </c>
-      <c r="F572" s="1" t="s">
-        <v>17</v>
+      <c r="F572" s="1">
+        <v>0</v>
       </c>
       <c r="G572" s="1">
         <v>1</v>
@@ -25960,8 +25960,8 @@
       <c r="I572" s="1">
         <v>4</v>
       </c>
-      <c r="J572" s="1" t="s">
-        <v>17</v>
+      <c r="J572" s="1">
+        <v>0</v>
       </c>
       <c r="K572" s="1">
         <v>1</v>
@@ -25992,8 +25992,8 @@
       <c r="E573" s="1">
         <v>4</v>
       </c>
-      <c r="F573" s="1" t="s">
-        <v>17</v>
+      <c r="F573" s="1">
+        <v>0</v>
       </c>
       <c r="G573" s="1">
         <v>1</v>
@@ -26004,8 +26004,8 @@
       <c r="I573" s="1">
         <v>4</v>
       </c>
-      <c r="J573" s="1" t="s">
-        <v>17</v>
+      <c r="J573" s="1">
+        <v>0</v>
       </c>
       <c r="K573" s="1">
         <v>1</v>
@@ -26036,8 +26036,8 @@
       <c r="E574" s="1">
         <v>4</v>
       </c>
-      <c r="F574" s="1" t="s">
-        <v>17</v>
+      <c r="F574" s="1">
+        <v>0</v>
       </c>
       <c r="G574" s="1">
         <v>1</v>
@@ -26048,8 +26048,8 @@
       <c r="I574" s="1">
         <v>4</v>
       </c>
-      <c r="J574" s="1" t="s">
-        <v>17</v>
+      <c r="J574" s="1">
+        <v>0</v>
       </c>
       <c r="K574" s="1">
         <v>1</v>

</xml_diff>